<commit_message>
Add 2021 and 2022 ICS values
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888B0960-C385-440A-8A26-CA8306C0F39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2847EB5-863D-4FF4-AF2B-67825FF84901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>US+MX</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2021 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2022 (AF)</t>
   </si>
 </sst>
 </file>
@@ -318,7 +324,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -369,6 +375,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -653,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -741,270 +751,288 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="19">
-        <v>598742</v>
-      </c>
-      <c r="C7" s="19">
-        <v>1375871</v>
-      </c>
-      <c r="D7" s="19">
-        <v>865741</v>
+    <row r="7" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="25">
+        <v>753423</v>
+      </c>
+      <c r="C7" s="25">
+        <v>1245693</v>
+      </c>
+      <c r="D7" s="25">
+        <v>1038765</v>
       </c>
       <c r="E7" s="19">
-        <f>41000+E8</f>
-        <v>173975</v>
+        <f>30000+E8</f>
+        <v>244975</v>
       </c>
       <c r="F7" s="2">
-        <f>SUM(B7:D7)</f>
-        <v>2840354</v>
+        <f t="shared" ref="F7:F8" si="0">SUM(B7:D7)</f>
+        <v>3037881</v>
       </c>
       <c r="G7" s="20">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="H7" s="11">
         <f>F7-F8</f>
-        <v>527727</v>
+        <v>46937</v>
       </c>
       <c r="I7" s="18">
-        <f t="shared" ref="I7:L8" si="0">B7-B8</f>
-        <v>125238</v>
+        <f t="shared" ref="I7:I8" si="1">B7-B8</f>
+        <v>69222</v>
       </c>
       <c r="J7" s="18">
+        <f t="shared" ref="J7:J8" si="2">C7-C8</f>
+        <v>-111392</v>
+      </c>
+      <c r="K7" s="18">
+        <f t="shared" ref="K7:K8" si="3">D7-D8</f>
+        <v>89107</v>
+      </c>
+      <c r="L7" s="18">
+        <f t="shared" ref="L7:L8" si="4">E7-E8</f>
+        <v>30000</v>
+      </c>
+      <c r="M7"/>
+      <c r="N7" s="11">
+        <f t="shared" ref="N7:N8" si="5">SUM(E7:F7)</f>
+        <v>3282856</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="25">
+        <v>684201</v>
+      </c>
+      <c r="C8" s="25">
+        <v>1357085</v>
+      </c>
+      <c r="D8" s="25">
+        <v>949658</v>
+      </c>
+      <c r="E8" s="19">
+        <f>41000+E9</f>
+        <v>214975</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>322661</v>
-      </c>
-      <c r="K7" s="18">
-        <f t="shared" si="0"/>
-        <v>79828</v>
-      </c>
-      <c r="L7" s="18">
-        <f t="shared" si="0"/>
+        <v>2990944</v>
+      </c>
+      <c r="G8" s="20">
+        <v>2021</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" ref="H7:H8" si="6">F8-F9</f>
+        <v>150590</v>
+      </c>
+      <c r="I8" s="18">
+        <f t="shared" si="1"/>
+        <v>85459</v>
+      </c>
+      <c r="J8" s="18">
+        <f t="shared" si="2"/>
+        <v>-18786</v>
+      </c>
+      <c r="K8" s="18">
+        <f t="shared" si="3"/>
+        <v>83917</v>
+      </c>
+      <c r="L8" s="18">
+        <f t="shared" si="4"/>
         <v>41000</v>
       </c>
-      <c r="N7" s="11">
-        <f>SUM(E7:F7)</f>
-        <v>3014329</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G8,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>473504</v>
-      </c>
-      <c r="C8" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G8,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>1053210</v>
-      </c>
-      <c r="D8" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G8,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>785913</v>
-      </c>
-      <c r="E8" s="2">
-        <v>132975</v>
-      </c>
-      <c r="F8" s="2">
-        <f>SUM(B8:D8)</f>
-        <v>2312627</v>
-      </c>
-      <c r="G8" s="12">
-        <v>2019</v>
-      </c>
-      <c r="H8" s="11">
-        <f>F8-F9</f>
-        <v>570695</v>
-      </c>
-      <c r="I8" s="18">
-        <f t="shared" si="0"/>
-        <v>130452</v>
-      </c>
-      <c r="J8" s="18">
-        <f t="shared" si="0"/>
-        <v>354778</v>
-      </c>
-      <c r="K8" s="18">
-        <f t="shared" si="0"/>
-        <v>85465</v>
-      </c>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18">
-        <f>H8-H7</f>
-        <v>42968</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M8"/>
+      <c r="N8" s="11">
+        <f t="shared" si="5"/>
+        <v>3205919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G9,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>343052</v>
-      </c>
-      <c r="C9" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G9,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>698432</v>
-      </c>
-      <c r="D9" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G9,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>700448</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B9" s="19">
+        <v>598742</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1375871</v>
+      </c>
+      <c r="D9" s="19">
+        <v>865741</v>
+      </c>
+      <c r="E9" s="19">
+        <f>41000+E10</f>
+        <v>173975</v>
+      </c>
       <c r="F9" s="2">
         <f>SUM(B9:D9)</f>
-        <v>1741932</v>
-      </c>
-      <c r="G9" s="9">
-        <v>2018</v>
+        <v>2840354</v>
+      </c>
+      <c r="G9" s="20">
+        <v>2020</v>
       </c>
       <c r="H9" s="11">
         <f>F9-F10</f>
-        <v>480441</v>
+        <v>527727</v>
       </c>
       <c r="I9" s="18">
-        <f t="shared" ref="I9:I16" si="1">B9-B10</f>
-        <v>216252</v>
+        <f t="shared" ref="I9:L10" si="7">B9-B10</f>
+        <v>125238</v>
       </c>
       <c r="J9" s="18">
-        <f t="shared" ref="J9:J16" si="2">C9-C10</f>
-        <v>146054</v>
+        <f t="shared" si="7"/>
+        <v>322661</v>
       </c>
       <c r="K9" s="18">
-        <f t="shared" ref="K9:K16" si="3">D9-D10</f>
-        <v>118135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+        <f t="shared" si="7"/>
+        <v>79828</v>
+      </c>
+      <c r="L9" s="18">
+        <f t="shared" si="7"/>
+        <v>41000</v>
+      </c>
+      <c r="N9" s="11">
+        <f>SUM(E9:F9)</f>
+        <v>3014329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>126800</v>
+        <v>473504</v>
       </c>
       <c r="C10" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>552378</v>
+        <v>1053210</v>
       </c>
       <c r="D10" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>582313</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>785913</v>
+      </c>
+      <c r="E10" s="2">
+        <v>132975</v>
+      </c>
       <c r="F10" s="2">
         <f>SUM(B10:D10)</f>
-        <v>1261491</v>
-      </c>
-      <c r="G10" s="10">
-        <v>2017</v>
+        <v>2312627</v>
+      </c>
+      <c r="G10" s="12">
+        <v>2019</v>
       </c>
       <c r="H10" s="11">
-        <f t="shared" ref="H10:H16" si="4">F10-F11</f>
-        <v>511813</v>
+        <f>F10-F11</f>
+        <v>570695</v>
       </c>
       <c r="I10" s="18">
-        <f t="shared" si="1"/>
-        <v>23750</v>
+        <f t="shared" si="7"/>
+        <v>130452</v>
       </c>
       <c r="J10" s="18">
-        <f t="shared" si="2"/>
-        <v>437312</v>
+        <f t="shared" si="7"/>
+        <v>354778</v>
       </c>
       <c r="K10" s="18">
-        <f t="shared" si="3"/>
-        <v>50751</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+        <f t="shared" si="7"/>
+        <v>85465</v>
+      </c>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18">
+        <f>H10-H9</f>
+        <v>42968</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <v>343052</v>
       </c>
       <c r="C11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>115066</v>
+        <v>698432</v>
       </c>
       <c r="D11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>531562</v>
+        <v>700448</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
-        <f t="shared" ref="F11:F17" si="5">SUM(B11:D11)</f>
-        <v>749678</v>
-      </c>
-      <c r="G11" s="10">
-        <v>2016</v>
+        <f>SUM(B11:D11)</f>
+        <v>1741932</v>
+      </c>
+      <c r="G11" s="9">
+        <v>2018</v>
       </c>
       <c r="H11" s="11">
-        <f t="shared" si="4"/>
-        <v>37814</v>
+        <f>F11-F12</f>
+        <v>480441</v>
       </c>
       <c r="I11" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="I11:I18" si="8">B11-B12</f>
+        <v>216252</v>
       </c>
       <c r="J11" s="18">
-        <f t="shared" si="2"/>
-        <v>17275</v>
+        <f t="shared" ref="J11:J18" si="9">C11-C12</f>
+        <v>146054</v>
       </c>
       <c r="K11" s="18">
-        <f t="shared" si="3"/>
-        <v>20539</v>
+        <f t="shared" ref="K11:K18" si="10">D11-D12</f>
+        <v>118135</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <v>126800</v>
       </c>
       <c r="C12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>97791</v>
+        <v>552378</v>
       </c>
       <c r="D12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>511023</v>
+        <v>582313</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
-        <f t="shared" si="5"/>
-        <v>711864</v>
+        <f>SUM(B12:D12)</f>
+        <v>1261491</v>
       </c>
       <c r="G12" s="10">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="H12" s="11">
-        <f t="shared" si="4"/>
-        <v>-125036</v>
+        <f t="shared" ref="H12:H18" si="11">F12-F13</f>
+        <v>511813</v>
       </c>
       <c r="I12" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>23750</v>
       </c>
       <c r="J12" s="18">
-        <f t="shared" si="2"/>
-        <v>-71294</v>
+        <f t="shared" si="9"/>
+        <v>437312</v>
       </c>
       <c r="K12" s="18">
-        <f t="shared" si="3"/>
-        <v>-53742</v>
+        <f t="shared" si="10"/>
+        <v>50751</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1012,40 +1040,40 @@
       </c>
       <c r="C13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>169085</v>
+        <v>115066</v>
       </c>
       <c r="D13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>564765</v>
+        <v>531562</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
-        <f t="shared" si="5"/>
-        <v>836900</v>
+        <f t="shared" ref="F13:F19" si="12">SUM(B13:D13)</f>
+        <v>749678</v>
       </c>
       <c r="G13" s="10">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="H13" s="11">
-        <f t="shared" si="4"/>
-        <v>-281264</v>
+        <f t="shared" si="11"/>
+        <v>37814</v>
       </c>
       <c r="I13" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J13" s="18">
-        <f t="shared" si="2"/>
-        <v>-304978</v>
+        <f t="shared" si="9"/>
+        <v>17275</v>
       </c>
       <c r="K13" s="18">
-        <f t="shared" si="3"/>
-        <v>23714</v>
+        <f t="shared" si="10"/>
+        <v>20539</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1053,40 +1081,40 @@
       </c>
       <c r="C14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>474063</v>
+        <v>97791</v>
       </c>
       <c r="D14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>541051</v>
+        <v>511023</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
-        <f t="shared" si="5"/>
-        <v>1118164</v>
+        <f t="shared" si="12"/>
+        <v>711864</v>
       </c>
       <c r="G14" s="10">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="H14" s="11">
-        <f t="shared" si="4"/>
-        <v>-77476</v>
+        <f t="shared" si="11"/>
+        <v>-125036</v>
       </c>
       <c r="I14" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J14" s="18">
-        <f t="shared" si="2"/>
-        <v>-105723</v>
+        <f t="shared" si="9"/>
+        <v>-71294</v>
       </c>
       <c r="K14" s="18">
-        <f t="shared" si="3"/>
-        <v>28247</v>
+        <f t="shared" si="10"/>
+        <v>-53742</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1094,40 +1122,40 @@
       </c>
       <c r="C15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>579786</v>
+        <v>169085</v>
       </c>
       <c r="D15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>512804</v>
+        <v>564765</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
-        <f t="shared" si="5"/>
-        <v>1195640</v>
+        <f t="shared" si="12"/>
+        <v>836900</v>
       </c>
       <c r="G15" s="10">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="H15" s="11">
-        <f t="shared" si="4"/>
-        <v>169240</v>
+        <f t="shared" si="11"/>
+        <v>-281264</v>
       </c>
       <c r="I15" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J15" s="18">
-        <f t="shared" si="2"/>
-        <v>139108</v>
+        <f t="shared" si="9"/>
+        <v>-304978</v>
       </c>
       <c r="K15" s="18">
-        <f t="shared" si="3"/>
-        <v>30132</v>
+        <f t="shared" si="10"/>
+        <v>23714</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1135,284 +1163,366 @@
       </c>
       <c r="C16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>440678</v>
+        <v>474063</v>
       </c>
       <c r="D16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>482672</v>
+        <v>541051</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2">
-        <f t="shared" si="5"/>
-        <v>1026400</v>
+        <f t="shared" si="12"/>
+        <v>1118164</v>
       </c>
       <c r="G16" s="10">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="H16" s="11">
-        <f t="shared" si="4"/>
-        <v>211059</v>
+        <f t="shared" si="11"/>
+        <v>-77476</v>
       </c>
       <c r="I16" s="18">
-        <f t="shared" si="1"/>
-        <v>956</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="J16" s="18">
-        <f t="shared" si="2"/>
-        <v>178688</v>
+        <f t="shared" si="9"/>
+        <v>-105723</v>
       </c>
       <c r="K16" s="18">
-        <f t="shared" si="3"/>
-        <v>31415</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="10"/>
+        <v>28247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>102094</v>
+        <v>103050</v>
       </c>
       <c r="C17" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>261990</v>
+        <v>579786</v>
       </c>
       <c r="D17" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>451257</v>
+        <v>512804</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2">
-        <f t="shared" si="5"/>
-        <v>815341</v>
+        <f t="shared" si="12"/>
+        <v>1195640</v>
       </c>
       <c r="G17" s="10">
-        <v>2010</v>
-      </c>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>2012</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="11"/>
+        <v>169240</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" si="9"/>
+        <v>139108</v>
+      </c>
+      <c r="K17" s="18">
+        <f t="shared" si="10"/>
+        <v>30132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2">
-        <v>100000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>103050</v>
       </c>
       <c r="C18" s="2">
-        <v>400000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>440678</v>
       </c>
       <c r="D18" s="2">
-        <v>125000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>482672</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2">
-        <f t="shared" ref="F18:F20" si="6">SUM(B18:D18)</f>
-        <v>625000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="12"/>
+        <v>1026400</v>
+      </c>
+      <c r="G18" s="10">
+        <v>2011</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="11"/>
+        <v>211059</v>
+      </c>
+      <c r="I18" s="18">
+        <f t="shared" si="8"/>
+        <v>956</v>
+      </c>
+      <c r="J18" s="18">
+        <f t="shared" si="9"/>
+        <v>178688</v>
+      </c>
+      <c r="K18" s="18">
+        <f t="shared" si="10"/>
+        <v>31415</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>102094</v>
       </c>
       <c r="C19" s="2">
-        <v>1500000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>261990</v>
       </c>
       <c r="D19" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>451257</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
-        <f t="shared" si="6"/>
-        <v>2100000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="12"/>
+        <v>815341</v>
+      </c>
+      <c r="G19" s="10">
+        <v>2010</v>
+      </c>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2">
-        <v>300000</v>
+        <v>100000</v>
       </c>
       <c r="C20" s="2">
         <v>400000</v>
       </c>
       <c r="D20" s="2">
-        <v>300000</v>
+        <v>125000</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="F20:F22" si="13">SUM(B20:D20)</f>
+        <v>625000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1500000</v>
+      </c>
+      <c r="D21" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2">
+        <f t="shared" si="13"/>
+        <v>2100000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C22" s="2">
+        <v>400000</v>
+      </c>
+      <c r="D22" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="8" t="str">
+      <c r="B25" s="8" t="str">
         <f>B6</f>
         <v>Arizona</v>
       </c>
-      <c r="C23" s="8" t="str">
-        <f t="shared" ref="C23:F23" si="7">C6</f>
+      <c r="C25" s="8" t="str">
+        <f t="shared" ref="C25:F25" si="14">C6</f>
         <v>California</v>
       </c>
-      <c r="D23" s="8" t="str">
-        <f t="shared" si="7"/>
+      <c r="D25" s="8" t="str">
+        <f t="shared" si="14"/>
         <v>Nevada</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8" t="str">
-        <f t="shared" si="7"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8" t="str">
+        <f t="shared" si="14"/>
         <v>Total</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B26" s="6">
         <v>100000</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C26" s="6">
         <v>400000</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D26" s="6">
         <v>125000</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6">
-        <f t="shared" ref="F24:F26" si="8">SUM(B24:D24)</f>
-        <v>625000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="6">
-        <v>500000</v>
-      </c>
-      <c r="C25" s="6">
-        <v>1700000</v>
-      </c>
-      <c r="D25" s="6">
-        <v>500000</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6">
-        <f t="shared" si="8"/>
-        <v>2700000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="6">
-        <f>B20</f>
-        <v>300000</v>
-      </c>
-      <c r="C26" s="6">
-        <f t="shared" ref="C26:D26" si="9">C20</f>
-        <v>400000</v>
-      </c>
-      <c r="D26" s="6">
-        <f t="shared" si="9"/>
-        <v>300000</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="F26:F28" si="15">SUM(B26:D26)</f>
+        <v>625000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="6">
+        <v>500000</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1700000</v>
+      </c>
+      <c r="D27" s="6">
+        <v>500000</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6">
+        <f t="shared" si="15"/>
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="6">
+        <f>B22</f>
+        <v>300000</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" ref="C28:D28" si="16">C22</f>
+        <v>400000</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" si="16"/>
+        <v>300000</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6">
+        <f t="shared" si="15"/>
         <v>1000000</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="21" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B33" s="4">
         <v>0.05</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C33" s="4">
         <v>0.05</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D33" s="4">
         <v>0.05</v>
       </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B34" s="4">
         <v>0.03</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C34" s="4">
         <v>0.03</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D34" s="4">
         <v>0.03</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E34" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A29:F29"/>
     <mergeCell ref="H5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1423,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1532,30 +1642,30 @@
         <v>8000</v>
       </c>
       <c r="E7" s="15">
-        <f>Sheet1!B$7/B7</f>
+        <f>Sheet1!B$9/B7</f>
         <v>3.1184479166666668</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15">
-        <f>Sheet1!D$7/D7</f>
+        <f>Sheet1!D$9/D7</f>
         <v>108.217625</v>
       </c>
       <c r="H7" s="17">
-        <f>Sheet1!B$26/ICStoDCP!B7</f>
+        <f>Sheet1!B$28/ICStoDCP!B7</f>
         <v>1.5625</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17">
-        <f>Sheet1!D$26/ICStoDCP!D7</f>
+        <f>Sheet1!D$28/ICStoDCP!D7</f>
         <v>37.5</v>
       </c>
       <c r="K7" s="16">
-        <f>Sheet1!B$24/ICStoDCP!B7</f>
+        <f>Sheet1!B$26/ICStoDCP!B7</f>
         <v>0.52083333333333337</v>
       </c>
       <c r="L7" s="16"/>
       <c r="M7" s="16">
-        <f>Sheet1!D$24/ICStoDCP!D7</f>
+        <f>Sheet1!D$26/ICStoDCP!D7</f>
         <v>15.625</v>
       </c>
     </row>
@@ -1571,30 +1681,30 @@
         <v>21000</v>
       </c>
       <c r="E8" s="15">
-        <f>Sheet1!B$7/B8</f>
+        <f>Sheet1!B$9/B8</f>
         <v>1.1694179687499999</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15">
-        <f>Sheet1!D$7/D8</f>
+        <f>Sheet1!D$9/D8</f>
         <v>41.225761904761903</v>
       </c>
       <c r="H8" s="17">
-        <f>Sheet1!B$26/ICStoDCP!B8</f>
+        <f>Sheet1!B$28/ICStoDCP!B8</f>
         <v>0.5859375</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17">
-        <f>Sheet1!D$26/ICStoDCP!D8</f>
+        <f>Sheet1!D$28/ICStoDCP!D8</f>
         <v>14.285714285714286</v>
       </c>
       <c r="K8" s="16">
-        <f>Sheet1!B$24/ICStoDCP!B8</f>
+        <f>Sheet1!B$26/ICStoDCP!B8</f>
         <v>0.1953125</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="16">
-        <f>Sheet1!D$24/ICStoDCP!D8</f>
+        <f>Sheet1!D$26/ICStoDCP!D8</f>
         <v>5.9523809523809526</v>
       </c>
     </row>
@@ -1610,30 +1720,30 @@
         <v>25000</v>
       </c>
       <c r="E9" s="15">
-        <f>Sheet1!B$7/B9</f>
+        <f>Sheet1!B$9/B9</f>
         <v>1.0113885135135134</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15">
-        <f>Sheet1!D$7/D9</f>
+        <f>Sheet1!D$9/D9</f>
         <v>34.629640000000002</v>
       </c>
       <c r="H9" s="17">
-        <f>Sheet1!B$26/ICStoDCP!B9</f>
+        <f>Sheet1!B$28/ICStoDCP!B9</f>
         <v>0.5067567567567568</v>
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17">
-        <f>Sheet1!D$26/ICStoDCP!D9</f>
+        <f>Sheet1!D$28/ICStoDCP!D9</f>
         <v>12</v>
       </c>
       <c r="K9" s="16">
-        <f>Sheet1!B$24/ICStoDCP!B9</f>
+        <f>Sheet1!B$26/ICStoDCP!B9</f>
         <v>0.16891891891891891</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16">
-        <f>Sheet1!D$24/ICStoDCP!D9</f>
+        <f>Sheet1!D$26/ICStoDCP!D9</f>
         <v>5</v>
       </c>
     </row>
@@ -1651,39 +1761,39 @@
         <v>27000</v>
       </c>
       <c r="E10" s="15">
-        <f>Sheet1!B$7/B10</f>
+        <f>Sheet1!B$9/B10</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F10" s="15">
-        <f>Sheet1!C$7/C10</f>
+        <f>Sheet1!C$9/C10</f>
         <v>6.8793550000000003</v>
       </c>
       <c r="G10" s="15">
-        <f>Sheet1!D$7/D10</f>
+        <f>Sheet1!D$9/D10</f>
         <v>32.064481481481479</v>
       </c>
       <c r="H10" s="17">
+        <f>Sheet1!B$28/ICStoDCP!B10</f>
+        <v>0.46875</v>
+      </c>
+      <c r="I10" s="17">
+        <f>Sheet1!C$28/ICStoDCP!C10</f>
+        <v>2</v>
+      </c>
+      <c r="J10" s="17">
+        <f>Sheet1!D$28/ICStoDCP!D10</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="K10" s="16">
         <f>Sheet1!B$26/ICStoDCP!B10</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I10" s="17">
+        <v>0.15625</v>
+      </c>
+      <c r="L10" s="16">
         <f>Sheet1!C$26/ICStoDCP!C10</f>
         <v>2</v>
       </c>
-      <c r="J10" s="17">
+      <c r="M10" s="16">
         <f>Sheet1!D$26/ICStoDCP!D10</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K10" s="16">
-        <f>Sheet1!B$24/ICStoDCP!B10</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L10" s="16">
-        <f>Sheet1!C$24/ICStoDCP!C10</f>
-        <v>2</v>
-      </c>
-      <c r="M10" s="16">
-        <f>Sheet1!D$24/ICStoDCP!D10</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1701,39 +1811,39 @@
         <v>27000</v>
       </c>
       <c r="E11" s="15">
-        <f>Sheet1!B$7/B11</f>
+        <f>Sheet1!B$9/B11</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F11" s="15">
-        <f>Sheet1!C$7/C11</f>
+        <f>Sheet1!C$9/C11</f>
         <v>5.5034840000000003</v>
       </c>
       <c r="G11" s="15">
-        <f>Sheet1!D$7/D11</f>
+        <f>Sheet1!D$9/D11</f>
         <v>32.064481481481479</v>
       </c>
       <c r="H11" s="17">
+        <f>Sheet1!B$28/ICStoDCP!B11</f>
+        <v>0.46875</v>
+      </c>
+      <c r="I11" s="17">
+        <f>Sheet1!C$28/ICStoDCP!C11</f>
+        <v>1.6</v>
+      </c>
+      <c r="J11" s="17">
+        <f>Sheet1!D$28/ICStoDCP!D11</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="K11" s="16">
         <f>Sheet1!B$26/ICStoDCP!B11</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I11" s="17">
+        <v>0.15625</v>
+      </c>
+      <c r="L11" s="16">
         <f>Sheet1!C$26/ICStoDCP!C11</f>
         <v>1.6</v>
       </c>
-      <c r="J11" s="17">
+      <c r="M11" s="16">
         <f>Sheet1!D$26/ICStoDCP!D11</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K11" s="16">
-        <f>Sheet1!B$24/ICStoDCP!B11</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L11" s="16">
-        <f>Sheet1!C$24/ICStoDCP!C11</f>
-        <v>1.6</v>
-      </c>
-      <c r="M11" s="16">
-        <f>Sheet1!D$24/ICStoDCP!D11</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1751,39 +1861,39 @@
         <v>27000</v>
       </c>
       <c r="E12" s="15">
-        <f>Sheet1!B$7/B12</f>
+        <f>Sheet1!B$9/B12</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F12" s="15">
-        <f>Sheet1!C$7/C12</f>
+        <f>Sheet1!C$9/C12</f>
         <v>4.5862366666666663</v>
       </c>
       <c r="G12" s="15">
-        <f>Sheet1!D$7/D12</f>
+        <f>Sheet1!D$9/D12</f>
         <v>32.064481481481479</v>
       </c>
       <c r="H12" s="17">
+        <f>Sheet1!B$28/ICStoDCP!B12</f>
+        <v>0.46875</v>
+      </c>
+      <c r="I12" s="17">
+        <f>Sheet1!C$28/ICStoDCP!C12</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="J12" s="17">
+        <f>Sheet1!D$28/ICStoDCP!D12</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="K12" s="16">
         <f>Sheet1!B$26/ICStoDCP!B12</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I12" s="17">
+        <v>0.15625</v>
+      </c>
+      <c r="L12" s="16">
         <f>Sheet1!C$26/ICStoDCP!C12</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="J12" s="17">
+      <c r="M12" s="16">
         <f>Sheet1!D$26/ICStoDCP!D12</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K12" s="16">
-        <f>Sheet1!B$24/ICStoDCP!B12</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L12" s="16">
-        <f>Sheet1!C$24/ICStoDCP!C12</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="M12" s="16">
-        <f>Sheet1!D$24/ICStoDCP!D12</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1801,39 +1911,39 @@
         <v>27000</v>
       </c>
       <c r="E13" s="15">
-        <f>Sheet1!B$7/B13</f>
+        <f>Sheet1!B$9/B13</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F13" s="15">
-        <f>Sheet1!C$7/C13</f>
+        <f>Sheet1!C$9/C13</f>
         <v>3.93106</v>
       </c>
       <c r="G13" s="15">
-        <f>Sheet1!D$7/D13</f>
+        <f>Sheet1!D$9/D13</f>
         <v>32.064481481481479</v>
       </c>
       <c r="H13" s="17">
+        <f>Sheet1!B$28/ICStoDCP!B13</f>
+        <v>0.46875</v>
+      </c>
+      <c r="I13" s="17">
+        <f>Sheet1!C$28/ICStoDCP!C13</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="J13" s="17">
+        <f>Sheet1!D$28/ICStoDCP!D13</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="K13" s="16">
         <f>Sheet1!B$26/ICStoDCP!B13</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I13" s="17">
+        <v>0.15625</v>
+      </c>
+      <c r="L13" s="16">
         <f>Sheet1!C$26/ICStoDCP!C13</f>
         <v>1.1428571428571428</v>
       </c>
-      <c r="J13" s="17">
+      <c r="M13" s="16">
         <f>Sheet1!D$26/ICStoDCP!D13</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K13" s="16">
-        <f>Sheet1!B$24/ICStoDCP!B13</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L13" s="16">
-        <f>Sheet1!C$24/ICStoDCP!C13</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="M13" s="16">
-        <f>Sheet1!D$24/ICStoDCP!D13</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1851,39 +1961,39 @@
         <v>30000</v>
       </c>
       <c r="E14" s="15">
-        <f>Sheet1!B$7/B14</f>
+        <f>Sheet1!B$9/B14</f>
         <v>0.83158611111111114</v>
       </c>
       <c r="F14" s="15">
-        <f>Sheet1!C$7/C14</f>
+        <f>Sheet1!C$9/C14</f>
         <v>3.93106</v>
       </c>
       <c r="G14" s="15">
-        <f>Sheet1!D$7/D14</f>
+        <f>Sheet1!D$9/D14</f>
         <v>28.858033333333335</v>
       </c>
       <c r="H14" s="17">
+        <f>Sheet1!B$28/ICStoDCP!B14</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I14" s="17">
+        <f>Sheet1!C$28/ICStoDCP!C14</f>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="J14" s="17">
+        <f>Sheet1!D$28/ICStoDCP!D14</f>
+        <v>10</v>
+      </c>
+      <c r="K14" s="16">
         <f>Sheet1!B$26/ICStoDCP!B14</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="I14" s="17">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="L14" s="16">
         <f>Sheet1!C$26/ICStoDCP!C14</f>
         <v>1.1428571428571428</v>
       </c>
-      <c r="J14" s="17">
+      <c r="M14" s="16">
         <f>Sheet1!D$26/ICStoDCP!D14</f>
-        <v>10</v>
-      </c>
-      <c r="K14" s="16">
-        <f>Sheet1!B$24/ICStoDCP!B14</f>
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="L14" s="16">
-        <f>Sheet1!C$24/ICStoDCP!C14</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="M14" s="16">
-        <f>Sheet1!D$24/ICStoDCP!D14</f>
         <v>4.166666666666667</v>
       </c>
     </row>
@@ -2042,7 +2152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:D42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix plots on Lake Mead Inflow; Add 2021 and 2022 to ICS code
Also write out dfICSBalanceMelt to csv file for use in later code
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2847EB5-863D-4FF4-AF2B-67825FF84901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8E3799-C0DB-4346-969F-18E8044ABD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -324,7 +324,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -375,10 +375,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -665,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -751,17 +747,17 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="12">
         <v>753423</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="12">
         <v>1245693</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="12">
         <v>1038765</v>
       </c>
       <c r="E7" s="19">
@@ -795,23 +791,22 @@
         <f t="shared" ref="L7:L8" si="4">E7-E8</f>
         <v>30000</v>
       </c>
-      <c r="M7"/>
       <c r="N7" s="11">
         <f t="shared" ref="N7:N8" si="5">SUM(E7:F7)</f>
         <v>3282856</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="12">
         <v>684201</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="12">
         <v>1357085</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="12">
         <v>949658</v>
       </c>
       <c r="E8" s="19">
@@ -826,7 +821,7 @@
         <v>2021</v>
       </c>
       <c r="H8" s="11">
-        <f t="shared" ref="H7:H8" si="6">F8-F9</f>
+        <f t="shared" ref="H8" si="6">F8-F9</f>
         <v>150590</v>
       </c>
       <c r="I8" s="18">
@@ -845,7 +840,6 @@
         <f t="shared" si="4"/>
         <v>41000</v>
       </c>
-      <c r="M8"/>
       <c r="N8" s="11">
         <f t="shared" si="5"/>
         <v>3205919</v>
@@ -1533,7 +1527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add ICS deposits to Lake Mead Inflow folder; read in + plot
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8E3799-C0DB-4346-969F-18E8044ABD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52421BA9-6EBE-41B9-83D5-CF62E7EEF365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update ICS to include 2022 and 2023 data
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52421BA9-6EBE-41B9-83D5-CF62E7EEF365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D357999-40C3-49F4-A416-4FC78D7CC8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-2640" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="ICStoDCP" sheetId="3" r:id="rId2"/>
-    <sheet name="DCPLogs" sheetId="4" r:id="rId3"/>
-    <sheet name="By User" sheetId="2" r:id="rId4"/>
+    <sheet name="Capacities" sheetId="5" r:id="rId2"/>
+    <sheet name="ICStoDCP" sheetId="3" r:id="rId3"/>
+    <sheet name="DCPLogs" sheetId="4" r:id="rId4"/>
+    <sheet name="By User" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="65">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -231,6 +232,9 @@
   </si>
   <si>
     <t>Balance - Dec 2022 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2023 (AF)</t>
   </si>
 </sst>
 </file>
@@ -324,7 +328,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -375,6 +379,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -659,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -747,327 +754,331 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="12">
-        <v>753423</v>
-      </c>
-      <c r="C7" s="12">
-        <v>1245693</v>
-      </c>
-      <c r="D7" s="12">
-        <v>1038765</v>
-      </c>
-      <c r="E7" s="19">
-        <f>30000+E8</f>
-        <v>244975</v>
+        <v>64</v>
+      </c>
+      <c r="B7" s="3">
+        <v>710589</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1661832</v>
+      </c>
+      <c r="D7" s="3">
+        <v>955543</v>
+      </c>
+      <c r="E7" s="24">
+        <f>E8-34000</f>
+        <v>210975</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" ref="F7:F8" si="0">SUM(B7:D7)</f>
-        <v>3037881</v>
-      </c>
-      <c r="G7" s="20">
-        <v>2022</v>
+        <f t="shared" ref="F7:F9" si="0">SUM(B7:D7)</f>
+        <v>3327964</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2023</v>
       </c>
       <c r="H7" s="11">
         <f>F7-F8</f>
-        <v>46937</v>
+        <v>290083</v>
       </c>
       <c r="I7" s="18">
-        <f t="shared" ref="I7:I8" si="1">B7-B8</f>
-        <v>69222</v>
+        <f t="shared" ref="I7" si="1">B7-B8</f>
+        <v>-42834</v>
       </c>
       <c r="J7" s="18">
-        <f t="shared" ref="J7:J8" si="2">C7-C8</f>
-        <v>-111392</v>
+        <f t="shared" ref="J7" si="2">C7-C8</f>
+        <v>416139</v>
       </c>
       <c r="K7" s="18">
-        <f t="shared" ref="K7:K8" si="3">D7-D8</f>
-        <v>89107</v>
+        <f t="shared" ref="K7" si="3">D7-D8</f>
+        <v>-83222</v>
       </c>
       <c r="L7" s="18">
-        <f t="shared" ref="L7:L8" si="4">E7-E8</f>
-        <v>30000</v>
-      </c>
-      <c r="N7" s="11">
-        <f t="shared" ref="N7:N8" si="5">SUM(E7:F7)</f>
-        <v>3282856</v>
+        <f t="shared" ref="L7" si="4">E7-E8</f>
+        <v>-34000</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B8" s="12">
-        <v>684201</v>
+        <v>753423</v>
       </c>
       <c r="C8" s="12">
-        <v>1357085</v>
+        <v>1245693</v>
       </c>
       <c r="D8" s="12">
-        <v>949658</v>
+        <v>1038765</v>
       </c>
       <c r="E8" s="19">
-        <f>41000+E9</f>
-        <v>214975</v>
+        <f>30000+E9</f>
+        <v>244975</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>2990944</v>
+        <v>3037881</v>
       </c>
       <c r="G8" s="20">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="H8" s="11">
-        <f t="shared" ref="H8" si="6">F8-F9</f>
-        <v>150590</v>
+        <f>F8-F9</f>
+        <v>46937</v>
       </c>
       <c r="I8" s="18">
-        <f t="shared" si="1"/>
-        <v>85459</v>
+        <f t="shared" ref="I8:I9" si="5">B8-B9</f>
+        <v>69222</v>
       </c>
       <c r="J8" s="18">
-        <f t="shared" si="2"/>
-        <v>-18786</v>
+        <f t="shared" ref="J8:J9" si="6">C8-C9</f>
+        <v>-111392</v>
       </c>
       <c r="K8" s="18">
-        <f t="shared" si="3"/>
-        <v>83917</v>
+        <f t="shared" ref="K8:K9" si="7">D8-D9</f>
+        <v>89107</v>
       </c>
       <c r="L8" s="18">
-        <f t="shared" si="4"/>
-        <v>41000</v>
+        <f t="shared" ref="L8:L9" si="8">E8-E9</f>
+        <v>30000</v>
       </c>
       <c r="N8" s="11">
-        <f t="shared" si="5"/>
-        <v>3205919</v>
+        <f t="shared" ref="N8:N9" si="9">SUM(E8:F8)</f>
+        <v>3282856</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="19">
-        <v>598742</v>
-      </c>
-      <c r="C9" s="19">
-        <v>1375871</v>
-      </c>
-      <c r="D9" s="19">
-        <v>865741</v>
+        <v>62</v>
+      </c>
+      <c r="B9" s="12">
+        <v>684201</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1357085</v>
+      </c>
+      <c r="D9" s="12">
+        <v>949658</v>
       </c>
       <c r="E9" s="19">
         <f>41000+E10</f>
-        <v>173975</v>
+        <v>214975</v>
       </c>
       <c r="F9" s="2">
-        <f>SUM(B9:D9)</f>
-        <v>2840354</v>
+        <f t="shared" si="0"/>
+        <v>2990944</v>
       </c>
       <c r="G9" s="20">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H9" s="11">
-        <f>F9-F10</f>
-        <v>527727</v>
+        <f t="shared" ref="H9" si="10">F9-F10</f>
+        <v>150590</v>
       </c>
       <c r="I9" s="18">
-        <f t="shared" ref="I9:L10" si="7">B9-B10</f>
-        <v>125238</v>
+        <f t="shared" si="5"/>
+        <v>85459</v>
       </c>
       <c r="J9" s="18">
-        <f t="shared" si="7"/>
-        <v>322661</v>
+        <f t="shared" si="6"/>
+        <v>-18786</v>
       </c>
       <c r="K9" s="18">
         <f t="shared" si="7"/>
-        <v>79828</v>
+        <v>83917</v>
       </c>
       <c r="L9" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>41000</v>
       </c>
       <c r="N9" s="11">
-        <f>SUM(E9:F9)</f>
-        <v>3014329</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="9"/>
+        <v>3205919</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>473504</v>
-      </c>
-      <c r="C10" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>1053210</v>
-      </c>
-      <c r="D10" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>785913</v>
-      </c>
-      <c r="E10" s="2">
-        <v>132975</v>
+        <v>51</v>
+      </c>
+      <c r="B10" s="19">
+        <v>598742</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1375871</v>
+      </c>
+      <c r="D10" s="19">
+        <v>865741</v>
+      </c>
+      <c r="E10" s="19">
+        <f>41000+E11</f>
+        <v>173975</v>
       </c>
       <c r="F10" s="2">
         <f>SUM(B10:D10)</f>
-        <v>2312627</v>
-      </c>
-      <c r="G10" s="12">
-        <v>2019</v>
+        <v>2840354</v>
+      </c>
+      <c r="G10" s="20">
+        <v>2020</v>
       </c>
       <c r="H10" s="11">
         <f>F10-F11</f>
-        <v>570695</v>
+        <v>527727</v>
       </c>
       <c r="I10" s="18">
-        <f t="shared" si="7"/>
-        <v>130452</v>
+        <f t="shared" ref="I10:L11" si="11">B10-B11</f>
+        <v>125238</v>
       </c>
       <c r="J10" s="18">
-        <f t="shared" si="7"/>
-        <v>354778</v>
+        <f t="shared" si="11"/>
+        <v>322661</v>
       </c>
       <c r="K10" s="18">
-        <f t="shared" si="7"/>
-        <v>85465</v>
-      </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18">
-        <f>H10-H9</f>
-        <v>42968</v>
+        <f t="shared" si="11"/>
+        <v>79828</v>
+      </c>
+      <c r="L10" s="18">
+        <f t="shared" si="11"/>
+        <v>41000</v>
+      </c>
+      <c r="N10" s="11">
+        <f>SUM(E10:F10)</f>
+        <v>3014329</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>343052</v>
+        <v>473504</v>
       </c>
       <c r="C11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>698432</v>
+        <v>1053210</v>
       </c>
       <c r="D11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>700448</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>785913</v>
+      </c>
+      <c r="E11" s="2">
+        <v>132975</v>
+      </c>
       <c r="F11" s="2">
         <f>SUM(B11:D11)</f>
-        <v>1741932</v>
-      </c>
-      <c r="G11" s="9">
-        <v>2018</v>
+        <v>2312627</v>
+      </c>
+      <c r="G11" s="12">
+        <v>2019</v>
       </c>
       <c r="H11" s="11">
         <f>F11-F12</f>
-        <v>480441</v>
+        <v>570695</v>
       </c>
       <c r="I11" s="18">
-        <f t="shared" ref="I11:I18" si="8">B11-B12</f>
-        <v>216252</v>
+        <f t="shared" si="11"/>
+        <v>130452</v>
       </c>
       <c r="J11" s="18">
-        <f t="shared" ref="J11:J18" si="9">C11-C12</f>
-        <v>146054</v>
+        <f t="shared" si="11"/>
+        <v>354778</v>
       </c>
       <c r="K11" s="18">
-        <f t="shared" ref="K11:K18" si="10">D11-D12</f>
-        <v>118135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <f t="shared" si="11"/>
+        <v>85465</v>
+      </c>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18">
+        <f>H11-H10</f>
+        <v>42968</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>126800</v>
+        <v>343052</v>
       </c>
       <c r="C12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>552378</v>
+        <v>698432</v>
       </c>
       <c r="D12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>582313</v>
+        <v>700448</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
         <f>SUM(B12:D12)</f>
-        <v>1261491</v>
-      </c>
-      <c r="G12" s="10">
-        <v>2017</v>
+        <v>1741932</v>
+      </c>
+      <c r="G12" s="9">
+        <v>2018</v>
       </c>
       <c r="H12" s="11">
-        <f t="shared" ref="H12:H18" si="11">F12-F13</f>
-        <v>511813</v>
+        <f>F12-F13</f>
+        <v>480441</v>
       </c>
       <c r="I12" s="18">
-        <f t="shared" si="8"/>
-        <v>23750</v>
+        <f t="shared" ref="I12:I19" si="12">B12-B13</f>
+        <v>216252</v>
       </c>
       <c r="J12" s="18">
-        <f t="shared" si="9"/>
-        <v>437312</v>
+        <f t="shared" ref="J12:J19" si="13">C12-C13</f>
+        <v>146054</v>
       </c>
       <c r="K12" s="18">
-        <f t="shared" si="10"/>
-        <v>50751</v>
+        <f t="shared" ref="K12:K19" si="14">D12-D13</f>
+        <v>118135</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <v>126800</v>
       </c>
       <c r="C13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>115066</v>
+        <v>552378</v>
       </c>
       <c r="D13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>531562</v>
+        <v>582313</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
-        <f t="shared" ref="F13:F19" si="12">SUM(B13:D13)</f>
-        <v>749678</v>
+        <f>SUM(B13:D13)</f>
+        <v>1261491</v>
       </c>
       <c r="G13" s="10">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="H13" s="11">
-        <f t="shared" si="11"/>
-        <v>37814</v>
+        <f t="shared" ref="H13:H19" si="15">F13-F14</f>
+        <v>511813</v>
       </c>
       <c r="I13" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>23750</v>
       </c>
       <c r="J13" s="18">
-        <f t="shared" si="9"/>
-        <v>17275</v>
+        <f t="shared" si="13"/>
+        <v>437312</v>
       </c>
       <c r="K13" s="18">
-        <f t="shared" si="10"/>
-        <v>20539</v>
+        <f t="shared" si="14"/>
+        <v>50751</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1075,40 +1086,40 @@
       </c>
       <c r="C14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>97791</v>
+        <v>115066</v>
       </c>
       <c r="D14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>511023</v>
+        <v>531562</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
+        <f t="shared" ref="F14:F20" si="16">SUM(B14:D14)</f>
+        <v>749678</v>
+      </c>
+      <c r="G14" s="10">
+        <v>2016</v>
+      </c>
+      <c r="H14" s="11">
+        <f t="shared" si="15"/>
+        <v>37814</v>
+      </c>
+      <c r="I14" s="18">
         <f t="shared" si="12"/>
-        <v>711864</v>
-      </c>
-      <c r="G14" s="10">
-        <v>2015</v>
-      </c>
-      <c r="H14" s="11">
-        <f t="shared" si="11"/>
-        <v>-125036</v>
-      </c>
-      <c r="I14" s="18">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J14" s="18">
-        <f t="shared" si="9"/>
-        <v>-71294</v>
+        <f t="shared" si="13"/>
+        <v>17275</v>
       </c>
       <c r="K14" s="18">
-        <f t="shared" si="10"/>
-        <v>-53742</v>
+        <f t="shared" si="14"/>
+        <v>20539</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1116,40 +1127,40 @@
       </c>
       <c r="C15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>169085</v>
+        <v>97791</v>
       </c>
       <c r="D15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>564765</v>
+        <v>511023</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
+        <f t="shared" si="16"/>
+        <v>711864</v>
+      </c>
+      <c r="G15" s="10">
+        <v>2015</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="15"/>
+        <v>-125036</v>
+      </c>
+      <c r="I15" s="18">
         <f t="shared" si="12"/>
-        <v>836900</v>
-      </c>
-      <c r="G15" s="10">
-        <v>2014</v>
-      </c>
-      <c r="H15" s="11">
-        <f t="shared" si="11"/>
-        <v>-281264</v>
-      </c>
-      <c r="I15" s="18">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J15" s="18">
-        <f t="shared" si="9"/>
-        <v>-304978</v>
+        <f t="shared" si="13"/>
+        <v>-71294</v>
       </c>
       <c r="K15" s="18">
-        <f t="shared" si="10"/>
-        <v>23714</v>
+        <f t="shared" si="14"/>
+        <v>-53742</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1157,40 +1168,40 @@
       </c>
       <c r="C16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>474063</v>
+        <v>169085</v>
       </c>
       <c r="D16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>541051</v>
+        <v>564765</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2">
+        <f t="shared" si="16"/>
+        <v>836900</v>
+      </c>
+      <c r="G16" s="10">
+        <v>2014</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="15"/>
+        <v>-281264</v>
+      </c>
+      <c r="I16" s="18">
         <f t="shared" si="12"/>
-        <v>1118164</v>
-      </c>
-      <c r="G16" s="10">
-        <v>2013</v>
-      </c>
-      <c r="H16" s="11">
-        <f t="shared" si="11"/>
-        <v>-77476</v>
-      </c>
-      <c r="I16" s="18">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J16" s="18">
-        <f t="shared" si="9"/>
-        <v>-105723</v>
+        <f t="shared" si="13"/>
+        <v>-304978</v>
       </c>
       <c r="K16" s="18">
-        <f t="shared" si="10"/>
-        <v>28247</v>
+        <f t="shared" si="14"/>
+        <v>23714</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1198,40 +1209,40 @@
       </c>
       <c r="C17" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>579786</v>
+        <v>474063</v>
       </c>
       <c r="D17" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>512804</v>
+        <v>541051</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2">
+        <f t="shared" si="16"/>
+        <v>1118164</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2013</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="15"/>
+        <v>-77476</v>
+      </c>
+      <c r="I17" s="18">
         <f t="shared" si="12"/>
-        <v>1195640</v>
-      </c>
-      <c r="G17" s="10">
-        <v>2012</v>
-      </c>
-      <c r="H17" s="11">
-        <f t="shared" si="11"/>
-        <v>169240</v>
-      </c>
-      <c r="I17" s="18">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J17" s="18">
-        <f t="shared" si="9"/>
-        <v>139108</v>
+        <f t="shared" si="13"/>
+        <v>-105723</v>
       </c>
       <c r="K17" s="18">
-        <f t="shared" si="10"/>
-        <v>30132</v>
+        <f t="shared" si="14"/>
+        <v>28247</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1239,131 +1250,165 @@
       </c>
       <c r="C18" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>440678</v>
+        <v>579786</v>
       </c>
       <c r="D18" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>482672</v>
+        <v>512804</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2">
+        <f t="shared" si="16"/>
+        <v>1195640</v>
+      </c>
+      <c r="G18" s="10">
+        <v>2012</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="15"/>
+        <v>169240</v>
+      </c>
+      <c r="I18" s="18">
         <f t="shared" si="12"/>
-        <v>1026400</v>
-      </c>
-      <c r="G18" s="10">
-        <v>2011</v>
-      </c>
-      <c r="H18" s="11">
-        <f t="shared" si="11"/>
-        <v>211059</v>
-      </c>
-      <c r="I18" s="18">
-        <f t="shared" si="8"/>
-        <v>956</v>
+        <v>0</v>
       </c>
       <c r="J18" s="18">
-        <f t="shared" si="9"/>
-        <v>178688</v>
+        <f t="shared" si="13"/>
+        <v>139108</v>
       </c>
       <c r="K18" s="18">
-        <f t="shared" si="10"/>
-        <v>31415</v>
+        <f t="shared" si="14"/>
+        <v>30132</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>102094</v>
+        <v>103050</v>
       </c>
       <c r="C19" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>261990</v>
+        <v>440678</v>
       </c>
       <c r="D19" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>451257</v>
+        <v>482672</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
+        <f t="shared" si="16"/>
+        <v>1026400</v>
+      </c>
+      <c r="G19" s="10">
+        <v>2011</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="15"/>
+        <v>211059</v>
+      </c>
+      <c r="I19" s="18">
         <f t="shared" si="12"/>
-        <v>815341</v>
-      </c>
-      <c r="G19" s="10">
-        <v>2010</v>
-      </c>
-      <c r="H19" s="11"/>
+        <v>956</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="13"/>
+        <v>178688</v>
+      </c>
+      <c r="K19" s="18">
+        <f t="shared" si="14"/>
+        <v>31415</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>100000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>102094</v>
       </c>
       <c r="C20" s="2">
-        <v>400000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>261990</v>
       </c>
       <c r="D20" s="2">
-        <v>125000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>451257</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
-        <f t="shared" ref="F20:F22" si="13">SUM(B20:D20)</f>
-        <v>625000</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>815341</v>
+      </c>
+      <c r="G20" s="10">
+        <v>2010</v>
+      </c>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="2">
-        <v>300000</v>
+        <v>100000</v>
       </c>
       <c r="C21" s="2">
-        <v>1500000</v>
+        <v>400000</v>
       </c>
       <c r="D21" s="2">
-        <v>300000</v>
+        <v>125000</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
-        <f t="shared" si="13"/>
-        <v>2100000</v>
+        <f t="shared" ref="F21:F23" si="17">SUM(B21:D21)</f>
+        <v>625000</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="2">
         <v>300000</v>
       </c>
       <c r="C22" s="2">
-        <v>400000</v>
+        <v>1500000</v>
       </c>
       <c r="D22" s="2">
         <v>300000</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2">
-        <f t="shared" si="13"/>
-        <v>1000000</v>
+        <f t="shared" si="17"/>
+        <v>2100000</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C23" s="2">
+        <v>400000</v>
+      </c>
+      <c r="D23" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <f t="shared" si="17"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1371,108 +1416,108 @@
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="7" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="8" t="str">
+      <c r="B26" s="8" t="str">
         <f>B6</f>
         <v>Arizona</v>
       </c>
-      <c r="C25" s="8" t="str">
-        <f t="shared" ref="C25:F25" si="14">C6</f>
+      <c r="C26" s="8" t="str">
+        <f t="shared" ref="C26:F26" si="18">C6</f>
         <v>California</v>
       </c>
-      <c r="D25" s="8" t="str">
-        <f t="shared" si="14"/>
+      <c r="D26" s="8" t="str">
+        <f t="shared" si="18"/>
         <v>Nevada</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8" t="str">
-        <f t="shared" si="14"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8" t="str">
+        <f t="shared" si="18"/>
         <v>Total</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="6">
-        <v>100000</v>
-      </c>
-      <c r="C26" s="6">
-        <v>400000</v>
-      </c>
-      <c r="D26" s="6">
-        <v>125000</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6">
-        <f t="shared" ref="F26:F28" si="15">SUM(B26:D26)</f>
-        <v>625000</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B27" s="6">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="C27" s="6">
-        <v>1700000</v>
+        <v>400000</v>
       </c>
       <c r="D27" s="6">
-        <v>500000</v>
+        <v>125000</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6">
-        <f t="shared" si="15"/>
-        <v>2700000</v>
+        <f t="shared" ref="F27:F29" si="19">SUM(B27:D27)</f>
+        <v>625000</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B28" s="6">
-        <f>B22</f>
-        <v>300000</v>
+        <v>500000</v>
       </c>
       <c r="C28" s="6">
-        <f t="shared" ref="C28:D28" si="16">C22</f>
-        <v>400000</v>
+        <v>1700000</v>
       </c>
       <c r="D28" s="6">
-        <f t="shared" si="16"/>
-        <v>300000</v>
+        <v>500000</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="6">
+        <f>B23</f>
+        <v>300000</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" ref="C29:D29" si="20">C23</f>
+        <v>400000</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" si="20"/>
+        <v>300000</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6">
+        <f t="shared" si="19"/>
         <v>1000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="21" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1480,43 +1525,50 @@
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="C33" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B35" s="4">
         <v>0.03</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C35" s="4">
         <v>0.03</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D35" s="4">
         <v>0.03</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
     <mergeCell ref="H5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1524,6 +1576,270 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9C09D6-2BEE-4EAC-9C47-48919B4DAC3E}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>400000</v>
+      </c>
+      <c r="D2" s="2">
+        <v>125000</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <f t="shared" ref="F2:F4" si="0">SUM(B2:D2)</f>
+        <v>625000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1500000</v>
+      </c>
+      <c r="D3" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <f t="shared" si="0"/>
+        <v>2100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>400000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>B1</f>
+        <v>Arizona</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f t="shared" ref="C7:F7" si="1">C1</f>
+        <v>California</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Nevada</v>
+      </c>
+      <c r="E7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Mexico</v>
+      </c>
+      <c r="F7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Total</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>100000</v>
+      </c>
+      <c r="C8" s="6">
+        <v>400000</v>
+      </c>
+      <c r="D8" s="6">
+        <v>125000</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
+        <f t="shared" ref="F8:F10" si="2">SUM(B8:D8)</f>
+        <v>625000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6">
+        <v>500000</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1700000</v>
+      </c>
+      <c r="D9" s="6">
+        <v>500000</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6">
+        <f t="shared" si="2"/>
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6">
+        <f>B4</f>
+        <v>300000</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" ref="C10:D10" si="3">C4</f>
+        <v>400000</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="3"/>
+        <v>300000</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
+        <f t="shared" si="2"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:F11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
   <dimension ref="A1:M14"/>
   <sheetViews>
@@ -1636,30 +1952,30 @@
         <v>8000</v>
       </c>
       <c r="E7" s="15">
-        <f>Sheet1!B$9/B7</f>
+        <f>Sheet1!B$10/B7</f>
         <v>3.1184479166666668</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15">
-        <f>Sheet1!D$9/D7</f>
+        <f>Sheet1!D$10/D7</f>
         <v>108.217625</v>
       </c>
       <c r="H7" s="17">
-        <f>Sheet1!B$28/ICStoDCP!B7</f>
+        <f>Sheet1!B$29/ICStoDCP!B7</f>
         <v>1.5625</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17">
-        <f>Sheet1!D$28/ICStoDCP!D7</f>
+        <f>Sheet1!D$29/ICStoDCP!D7</f>
         <v>37.5</v>
       </c>
       <c r="K7" s="16">
-        <f>Sheet1!B$26/ICStoDCP!B7</f>
+        <f>Sheet1!B$27/ICStoDCP!B7</f>
         <v>0.52083333333333337</v>
       </c>
       <c r="L7" s="16"/>
       <c r="M7" s="16">
-        <f>Sheet1!D$26/ICStoDCP!D7</f>
+        <f>Sheet1!D$27/ICStoDCP!D7</f>
         <v>15.625</v>
       </c>
     </row>
@@ -1675,30 +1991,30 @@
         <v>21000</v>
       </c>
       <c r="E8" s="15">
-        <f>Sheet1!B$9/B8</f>
+        <f>Sheet1!B$10/B8</f>
         <v>1.1694179687499999</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15">
-        <f>Sheet1!D$9/D8</f>
+        <f>Sheet1!D$10/D8</f>
         <v>41.225761904761903</v>
       </c>
       <c r="H8" s="17">
-        <f>Sheet1!B$28/ICStoDCP!B8</f>
+        <f>Sheet1!B$29/ICStoDCP!B8</f>
         <v>0.5859375</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17">
-        <f>Sheet1!D$28/ICStoDCP!D8</f>
+        <f>Sheet1!D$29/ICStoDCP!D8</f>
         <v>14.285714285714286</v>
       </c>
       <c r="K8" s="16">
-        <f>Sheet1!B$26/ICStoDCP!B8</f>
+        <f>Sheet1!B$27/ICStoDCP!B8</f>
         <v>0.1953125</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="16">
-        <f>Sheet1!D$26/ICStoDCP!D8</f>
+        <f>Sheet1!D$27/ICStoDCP!D8</f>
         <v>5.9523809523809526</v>
       </c>
     </row>
@@ -1714,30 +2030,30 @@
         <v>25000</v>
       </c>
       <c r="E9" s="15">
-        <f>Sheet1!B$9/B9</f>
+        <f>Sheet1!B$10/B9</f>
         <v>1.0113885135135134</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15">
-        <f>Sheet1!D$9/D9</f>
+        <f>Sheet1!D$10/D9</f>
         <v>34.629640000000002</v>
       </c>
       <c r="H9" s="17">
-        <f>Sheet1!B$28/ICStoDCP!B9</f>
+        <f>Sheet1!B$29/ICStoDCP!B9</f>
         <v>0.5067567567567568</v>
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17">
-        <f>Sheet1!D$28/ICStoDCP!D9</f>
+        <f>Sheet1!D$29/ICStoDCP!D9</f>
         <v>12</v>
       </c>
       <c r="K9" s="16">
-        <f>Sheet1!B$26/ICStoDCP!B9</f>
+        <f>Sheet1!B$27/ICStoDCP!B9</f>
         <v>0.16891891891891891</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16">
-        <f>Sheet1!D$26/ICStoDCP!D9</f>
+        <f>Sheet1!D$27/ICStoDCP!D9</f>
         <v>5</v>
       </c>
     </row>
@@ -1755,39 +2071,39 @@
         <v>27000</v>
       </c>
       <c r="E10" s="15">
-        <f>Sheet1!B$9/B10</f>
+        <f>Sheet1!B$10/B10</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F10" s="15">
-        <f>Sheet1!C$9/C10</f>
+        <f>Sheet1!C$10/C10</f>
         <v>6.8793550000000003</v>
       </c>
       <c r="G10" s="15">
-        <f>Sheet1!D$9/D10</f>
+        <f>Sheet1!D$10/D10</f>
         <v>32.064481481481479</v>
       </c>
       <c r="H10" s="17">
-        <f>Sheet1!B$28/ICStoDCP!B10</f>
+        <f>Sheet1!B$29/ICStoDCP!B10</f>
         <v>0.46875</v>
       </c>
       <c r="I10" s="17">
-        <f>Sheet1!C$28/ICStoDCP!C10</f>
+        <f>Sheet1!C$29/ICStoDCP!C10</f>
         <v>2</v>
       </c>
       <c r="J10" s="17">
-        <f>Sheet1!D$28/ICStoDCP!D10</f>
+        <f>Sheet1!D$29/ICStoDCP!D10</f>
         <v>11.111111111111111</v>
       </c>
       <c r="K10" s="16">
-        <f>Sheet1!B$26/ICStoDCP!B10</f>
+        <f>Sheet1!B$27/ICStoDCP!B10</f>
         <v>0.15625</v>
       </c>
       <c r="L10" s="16">
-        <f>Sheet1!C$26/ICStoDCP!C10</f>
+        <f>Sheet1!C$27/ICStoDCP!C10</f>
         <v>2</v>
       </c>
       <c r="M10" s="16">
-        <f>Sheet1!D$26/ICStoDCP!D10</f>
+        <f>Sheet1!D$27/ICStoDCP!D10</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1805,39 +2121,39 @@
         <v>27000</v>
       </c>
       <c r="E11" s="15">
-        <f>Sheet1!B$9/B11</f>
+        <f>Sheet1!B$10/B11</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F11" s="15">
-        <f>Sheet1!C$9/C11</f>
+        <f>Sheet1!C$10/C11</f>
         <v>5.5034840000000003</v>
       </c>
       <c r="G11" s="15">
-        <f>Sheet1!D$9/D11</f>
+        <f>Sheet1!D$10/D11</f>
         <v>32.064481481481479</v>
       </c>
       <c r="H11" s="17">
-        <f>Sheet1!B$28/ICStoDCP!B11</f>
+        <f>Sheet1!B$29/ICStoDCP!B11</f>
         <v>0.46875</v>
       </c>
       <c r="I11" s="17">
-        <f>Sheet1!C$28/ICStoDCP!C11</f>
+        <f>Sheet1!C$29/ICStoDCP!C11</f>
         <v>1.6</v>
       </c>
       <c r="J11" s="17">
-        <f>Sheet1!D$28/ICStoDCP!D11</f>
+        <f>Sheet1!D$29/ICStoDCP!D11</f>
         <v>11.111111111111111</v>
       </c>
       <c r="K11" s="16">
-        <f>Sheet1!B$26/ICStoDCP!B11</f>
+        <f>Sheet1!B$27/ICStoDCP!B11</f>
         <v>0.15625</v>
       </c>
       <c r="L11" s="16">
-        <f>Sheet1!C$26/ICStoDCP!C11</f>
+        <f>Sheet1!C$27/ICStoDCP!C11</f>
         <v>1.6</v>
       </c>
       <c r="M11" s="16">
-        <f>Sheet1!D$26/ICStoDCP!D11</f>
+        <f>Sheet1!D$27/ICStoDCP!D11</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1855,39 +2171,39 @@
         <v>27000</v>
       </c>
       <c r="E12" s="15">
-        <f>Sheet1!B$9/B12</f>
+        <f>Sheet1!B$10/B12</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F12" s="15">
-        <f>Sheet1!C$9/C12</f>
+        <f>Sheet1!C$10/C12</f>
         <v>4.5862366666666663</v>
       </c>
       <c r="G12" s="15">
-        <f>Sheet1!D$9/D12</f>
+        <f>Sheet1!D$10/D12</f>
         <v>32.064481481481479</v>
       </c>
       <c r="H12" s="17">
-        <f>Sheet1!B$28/ICStoDCP!B12</f>
+        <f>Sheet1!B$29/ICStoDCP!B12</f>
         <v>0.46875</v>
       </c>
       <c r="I12" s="17">
-        <f>Sheet1!C$28/ICStoDCP!C12</f>
+        <f>Sheet1!C$29/ICStoDCP!C12</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="J12" s="17">
-        <f>Sheet1!D$28/ICStoDCP!D12</f>
+        <f>Sheet1!D$29/ICStoDCP!D12</f>
         <v>11.111111111111111</v>
       </c>
       <c r="K12" s="16">
-        <f>Sheet1!B$26/ICStoDCP!B12</f>
+        <f>Sheet1!B$27/ICStoDCP!B12</f>
         <v>0.15625</v>
       </c>
       <c r="L12" s="16">
-        <f>Sheet1!C$26/ICStoDCP!C12</f>
+        <f>Sheet1!C$27/ICStoDCP!C12</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="M12" s="16">
-        <f>Sheet1!D$26/ICStoDCP!D12</f>
+        <f>Sheet1!D$27/ICStoDCP!D12</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1905,39 +2221,39 @@
         <v>27000</v>
       </c>
       <c r="E13" s="15">
-        <f>Sheet1!B$9/B13</f>
+        <f>Sheet1!B$10/B13</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F13" s="15">
-        <f>Sheet1!C$9/C13</f>
+        <f>Sheet1!C$10/C13</f>
         <v>3.93106</v>
       </c>
       <c r="G13" s="15">
-        <f>Sheet1!D$9/D13</f>
+        <f>Sheet1!D$10/D13</f>
         <v>32.064481481481479</v>
       </c>
       <c r="H13" s="17">
-        <f>Sheet1!B$28/ICStoDCP!B13</f>
+        <f>Sheet1!B$29/ICStoDCP!B13</f>
         <v>0.46875</v>
       </c>
       <c r="I13" s="17">
-        <f>Sheet1!C$28/ICStoDCP!C13</f>
+        <f>Sheet1!C$29/ICStoDCP!C13</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="J13" s="17">
-        <f>Sheet1!D$28/ICStoDCP!D13</f>
+        <f>Sheet1!D$29/ICStoDCP!D13</f>
         <v>11.111111111111111</v>
       </c>
       <c r="K13" s="16">
-        <f>Sheet1!B$26/ICStoDCP!B13</f>
+        <f>Sheet1!B$27/ICStoDCP!B13</f>
         <v>0.15625</v>
       </c>
       <c r="L13" s="16">
-        <f>Sheet1!C$26/ICStoDCP!C13</f>
+        <f>Sheet1!C$27/ICStoDCP!C13</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="M13" s="16">
-        <f>Sheet1!D$26/ICStoDCP!D13</f>
+        <f>Sheet1!D$27/ICStoDCP!D13</f>
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1955,39 +2271,39 @@
         <v>30000</v>
       </c>
       <c r="E14" s="15">
-        <f>Sheet1!B$9/B14</f>
+        <f>Sheet1!B$10/B14</f>
         <v>0.83158611111111114</v>
       </c>
       <c r="F14" s="15">
-        <f>Sheet1!C$9/C14</f>
+        <f>Sheet1!C$10/C14</f>
         <v>3.93106</v>
       </c>
       <c r="G14" s="15">
-        <f>Sheet1!D$9/D14</f>
+        <f>Sheet1!D$10/D14</f>
         <v>28.858033333333335</v>
       </c>
       <c r="H14" s="17">
-        <f>Sheet1!B$28/ICStoDCP!B14</f>
+        <f>Sheet1!B$29/ICStoDCP!B14</f>
         <v>0.41666666666666669</v>
       </c>
       <c r="I14" s="17">
-        <f>Sheet1!C$28/ICStoDCP!C14</f>
+        <f>Sheet1!C$29/ICStoDCP!C14</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="J14" s="17">
-        <f>Sheet1!D$28/ICStoDCP!D14</f>
+        <f>Sheet1!D$29/ICStoDCP!D14</f>
         <v>10</v>
       </c>
       <c r="K14" s="16">
-        <f>Sheet1!B$26/ICStoDCP!B14</f>
+        <f>Sheet1!B$27/ICStoDCP!B14</f>
         <v>0.1388888888888889</v>
       </c>
       <c r="L14" s="16">
-        <f>Sheet1!C$26/ICStoDCP!C14</f>
+        <f>Sheet1!C$27/ICStoDCP!C14</f>
         <v>1.1428571428571428</v>
       </c>
       <c r="M14" s="16">
-        <f>Sheet1!D$26/ICStoDCP!D14</f>
+        <f>Sheet1!D$27/ICStoDCP!D14</f>
         <v>4.166666666666667</v>
       </c>
     </row>
@@ -1999,7 +2315,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
   <dimension ref="A2:I7"/>
   <sheetViews>
@@ -2142,7 +2458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>

</xml_diff>

<commit_message>
Calculate ICS deposits to include exclude
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D357999-40C3-49F4-A416-4FC78D7CC8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0D349E-1B7B-4764-AC7A-7C5D7DAF6D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-2640" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -372,6 +372,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -379,9 +382,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,12 +706,12 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -767,7 +767,7 @@
       <c r="D7" s="3">
         <v>955543</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="21">
         <f>E8-34000</f>
         <v>210975</v>
       </c>
@@ -1505,14 +1505,14 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
@@ -1579,7 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9C09D6-2BEE-4EAC-9C47-48919B4DAC3E}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:F7"/>
     </sheetView>
   </sheetViews>
@@ -1770,14 +1770,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1855,11 +1855,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="H1" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Update ICS to go from 2007 to 2023
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0D349E-1B7B-4764-AC7A-7C5D7DAF6D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63C8CFF-592F-43FD-B532-430076367862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-2640" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="68">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>Balance - Dec 2023 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2009 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2008 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2007 (AF)</t>
   </si>
 </sst>
 </file>
@@ -666,10 +675,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,7 +938,7 @@
         <v>527727</v>
       </c>
       <c r="I10" s="18">
-        <f t="shared" ref="I10:L11" si="11">B10-B11</f>
+        <f t="shared" ref="I10:L23" si="11">B10-B11</f>
         <v>125238</v>
       </c>
       <c r="J10" s="18">
@@ -987,6 +999,10 @@
       <c r="K11" s="18">
         <f t="shared" si="11"/>
         <v>85465</v>
+      </c>
+      <c r="L11" s="18">
+        <f t="shared" si="11"/>
+        <v>132975</v>
       </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18">
@@ -1034,6 +1050,10 @@
         <f t="shared" ref="K12:K19" si="14">D12-D13</f>
         <v>118135</v>
       </c>
+      <c r="L12" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1075,6 +1095,10 @@
         <f t="shared" si="14"/>
         <v>50751</v>
       </c>
+      <c r="L13" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1094,7 +1118,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
-        <f t="shared" ref="F14:F20" si="16">SUM(B14:D14)</f>
+        <f t="shared" ref="F14:F23" si="16">SUM(B14:D14)</f>
         <v>749678</v>
       </c>
       <c r="G14" s="10">
@@ -1115,6 +1139,10 @@
       <c r="K14" s="18">
         <f t="shared" si="14"/>
         <v>20539</v>
+      </c>
+      <c r="L14" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1157,6 +1185,10 @@
         <f t="shared" si="14"/>
         <v>-53742</v>
       </c>
+      <c r="L15" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1198,8 +1230,12 @@
         <f t="shared" si="14"/>
         <v>23714</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1239,8 +1275,12 @@
         <f t="shared" si="14"/>
         <v>28247</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1280,8 +1320,12 @@
         <f t="shared" si="14"/>
         <v>30132</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1321,8 +1365,12 @@
         <f t="shared" si="14"/>
         <v>31415</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1346,229 +1394,157 @@
       <c r="G20" s="10">
         <v>2010</v>
       </c>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H20" s="11">
+        <f t="shared" ref="H20:H23" si="17">F20-F21</f>
+        <v>158151</v>
+      </c>
+      <c r="I20" s="18">
+        <f t="shared" ref="I20:I23" si="18">B20-B21</f>
+        <v>2094</v>
+      </c>
+      <c r="J20" s="18">
+        <f t="shared" ref="J20:J23" si="19">C20-C21</f>
+        <v>104800</v>
+      </c>
+      <c r="K20" s="18">
+        <f t="shared" ref="K20:K23" si="20">D20-D21</f>
+        <v>51257</v>
+      </c>
+      <c r="L20" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="B21" s="2">
         <v>100000</v>
       </c>
       <c r="C21" s="2">
+        <f>79790+66000+11400</f>
+        <v>157190</v>
+      </c>
+      <c r="D21" s="2">
         <v>400000</v>
-      </c>
-      <c r="D21" s="2">
-        <v>125000</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
-        <f t="shared" ref="F21:F23" si="17">SUM(B21:D21)</f>
-        <v>625000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" si="16"/>
+        <v>657190</v>
+      </c>
+      <c r="G21" s="10">
+        <v>2009</v>
+      </c>
+      <c r="H21" s="11">
+        <f t="shared" si="17"/>
+        <v>63617</v>
+      </c>
+      <c r="I21" s="18">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="18">
+        <f t="shared" si="19"/>
+        <v>63617</v>
+      </c>
+      <c r="K21" s="18">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2">
-        <v>300000</v>
+        <v>100000</v>
       </c>
       <c r="C22" s="2">
-        <v>1500000</v>
+        <f>27573+66000</f>
+        <v>93573</v>
       </c>
       <c r="D22" s="2">
-        <v>300000</v>
+        <v>400000</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2">
+        <f t="shared" si="16"/>
+        <v>593573</v>
+      </c>
+      <c r="G22" s="10">
+        <v>2008</v>
+      </c>
+      <c r="H22" s="11">
         <f t="shared" si="17"/>
-        <v>2100000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+        <v>552175</v>
+      </c>
+      <c r="I22" s="18">
+        <f t="shared" si="18"/>
+        <v>100000</v>
+      </c>
+      <c r="J22" s="18">
+        <f t="shared" si="19"/>
+        <v>52175</v>
+      </c>
+      <c r="K22" s="18">
+        <f t="shared" si="20"/>
+        <v>400000</v>
+      </c>
+      <c r="L22" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B23" s="2">
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2">
-        <v>400000</v>
+        <v>41398</v>
       </c>
       <c r="D23" s="2">
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2">
+        <f t="shared" si="16"/>
+        <v>41398</v>
+      </c>
+      <c r="G23" s="10">
+        <v>2007</v>
+      </c>
+      <c r="H23" s="11">
         <f t="shared" si="17"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="8" t="str">
-        <f>B6</f>
-        <v>Arizona</v>
-      </c>
-      <c r="C26" s="8" t="str">
-        <f t="shared" ref="C26:F26" si="18">C6</f>
-        <v>California</v>
-      </c>
-      <c r="D26" s="8" t="str">
+        <v>41398</v>
+      </c>
+      <c r="I23" s="18">
         <f t="shared" si="18"/>
-        <v>Nevada</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8" t="str">
-        <f t="shared" si="18"/>
-        <v>Total</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="6">
-        <v>100000</v>
-      </c>
-      <c r="C27" s="6">
-        <v>400000</v>
-      </c>
-      <c r="D27" s="6">
-        <v>125000</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6">
-        <f t="shared" ref="F27:F29" si="19">SUM(B27:D27)</f>
-        <v>625000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="6">
-        <v>500000</v>
-      </c>
-      <c r="C28" s="6">
-        <v>1700000</v>
-      </c>
-      <c r="D28" s="6">
-        <v>500000</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6">
+        <v>0</v>
+      </c>
+      <c r="J23" s="18">
         <f t="shared" si="19"/>
-        <v>2700000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="6">
-        <f>B23</f>
-        <v>300000</v>
-      </c>
-      <c r="C29" s="6">
-        <f t="shared" ref="C29:D29" si="20">C23</f>
-        <v>400000</v>
-      </c>
-      <c r="D29" s="6">
+        <v>41398</v>
+      </c>
+      <c r="K23" s="18">
         <f t="shared" si="20"/>
-        <v>300000</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6">
-        <f t="shared" si="19"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="C34" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="D34" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="C35" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="D35" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="E35" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A30:F30"/>
+  <mergeCells count="1">
     <mergeCell ref="H5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1580,7 +1556,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1960,23 +1936,23 @@
         <f>Sheet1!D$10/D7</f>
         <v>108.217625</v>
       </c>
-      <c r="H7" s="17">
-        <f>Sheet1!B$29/ICStoDCP!B7</f>
-        <v>1.5625</v>
+      <c r="H7" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B7</f>
+        <v>#REF!</v>
       </c>
       <c r="I7" s="17"/>
-      <c r="J7" s="17">
-        <f>Sheet1!D$29/ICStoDCP!D7</f>
-        <v>37.5</v>
-      </c>
-      <c r="K7" s="16">
-        <f>Sheet1!B$27/ICStoDCP!B7</f>
-        <v>0.52083333333333337</v>
+      <c r="J7" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D7</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K7" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B7</f>
+        <v>#REF!</v>
       </c>
       <c r="L7" s="16"/>
-      <c r="M7" s="16">
-        <f>Sheet1!D$27/ICStoDCP!D7</f>
-        <v>15.625</v>
+      <c r="M7" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D7</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -1999,23 +1975,23 @@
         <f>Sheet1!D$10/D8</f>
         <v>41.225761904761903</v>
       </c>
-      <c r="H8" s="17">
-        <f>Sheet1!B$29/ICStoDCP!B8</f>
-        <v>0.5859375</v>
+      <c r="H8" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B8</f>
+        <v>#REF!</v>
       </c>
       <c r="I8" s="17"/>
-      <c r="J8" s="17">
-        <f>Sheet1!D$29/ICStoDCP!D8</f>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="K8" s="16">
-        <f>Sheet1!B$27/ICStoDCP!B8</f>
-        <v>0.1953125</v>
+      <c r="J8" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K8" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B8</f>
+        <v>#REF!</v>
       </c>
       <c r="L8" s="16"/>
-      <c r="M8" s="16">
-        <f>Sheet1!D$27/ICStoDCP!D8</f>
-        <v>5.9523809523809526</v>
+      <c r="M8" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D8</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -2038,23 +2014,23 @@
         <f>Sheet1!D$10/D9</f>
         <v>34.629640000000002</v>
       </c>
-      <c r="H9" s="17">
-        <f>Sheet1!B$29/ICStoDCP!B9</f>
-        <v>0.5067567567567568</v>
+      <c r="H9" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B9</f>
+        <v>#REF!</v>
       </c>
       <c r="I9" s="17"/>
-      <c r="J9" s="17">
-        <f>Sheet1!D$29/ICStoDCP!D9</f>
-        <v>12</v>
-      </c>
-      <c r="K9" s="16">
-        <f>Sheet1!B$27/ICStoDCP!B9</f>
-        <v>0.16891891891891891</v>
+      <c r="J9" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D9</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K9" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B9</f>
+        <v>#REF!</v>
       </c>
       <c r="L9" s="16"/>
-      <c r="M9" s="16">
-        <f>Sheet1!D$27/ICStoDCP!D9</f>
-        <v>5</v>
+      <c r="M9" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D9</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -2082,29 +2058,29 @@
         <f>Sheet1!D$10/D10</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H10" s="17">
-        <f>Sheet1!B$29/ICStoDCP!B10</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I10" s="17">
-        <f>Sheet1!C$29/ICStoDCP!C10</f>
-        <v>2</v>
-      </c>
-      <c r="J10" s="17">
-        <f>Sheet1!D$29/ICStoDCP!D10</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K10" s="16">
-        <f>Sheet1!B$27/ICStoDCP!B10</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L10" s="16">
-        <f>Sheet1!C$27/ICStoDCP!C10</f>
-        <v>2</v>
-      </c>
-      <c r="M10" s="16">
-        <f>Sheet1!D$27/ICStoDCP!D10</f>
-        <v>4.6296296296296298</v>
+      <c r="H10" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I10" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J10" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K10" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L10" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M10" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D10</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -2132,29 +2108,29 @@
         <f>Sheet1!D$10/D11</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H11" s="17">
-        <f>Sheet1!B$29/ICStoDCP!B11</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I11" s="17">
-        <f>Sheet1!C$29/ICStoDCP!C11</f>
-        <v>1.6</v>
-      </c>
-      <c r="J11" s="17">
-        <f>Sheet1!D$29/ICStoDCP!D11</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K11" s="16">
-        <f>Sheet1!B$27/ICStoDCP!B11</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L11" s="16">
-        <f>Sheet1!C$27/ICStoDCP!C11</f>
-        <v>1.6</v>
-      </c>
-      <c r="M11" s="16">
-        <f>Sheet1!D$27/ICStoDCP!D11</f>
-        <v>4.6296296296296298</v>
+      <c r="H11" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I11" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J11" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K11" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L11" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M11" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D11</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -2182,29 +2158,29 @@
         <f>Sheet1!D$10/D12</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H12" s="17">
-        <f>Sheet1!B$29/ICStoDCP!B12</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I12" s="17">
-        <f>Sheet1!C$29/ICStoDCP!C12</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="J12" s="17">
-        <f>Sheet1!D$29/ICStoDCP!D12</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K12" s="16">
-        <f>Sheet1!B$27/ICStoDCP!B12</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L12" s="16">
-        <f>Sheet1!C$27/ICStoDCP!C12</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="M12" s="16">
-        <f>Sheet1!D$27/ICStoDCP!D12</f>
-        <v>4.6296296296296298</v>
+      <c r="H12" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I12" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J12" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K12" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L12" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M12" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D12</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -2232,29 +2208,29 @@
         <f>Sheet1!D$10/D13</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H13" s="17">
-        <f>Sheet1!B$29/ICStoDCP!B13</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I13" s="17">
-        <f>Sheet1!C$29/ICStoDCP!C13</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="J13" s="17">
-        <f>Sheet1!D$29/ICStoDCP!D13</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K13" s="16">
-        <f>Sheet1!B$27/ICStoDCP!B13</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L13" s="16">
-        <f>Sheet1!C$27/ICStoDCP!C13</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="M13" s="16">
-        <f>Sheet1!D$27/ICStoDCP!D13</f>
-        <v>4.6296296296296298</v>
+      <c r="H13" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I13" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J13" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K13" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L13" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M13" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D13</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -2282,29 +2258,29 @@
         <f>Sheet1!D$10/D14</f>
         <v>28.858033333333335</v>
       </c>
-      <c r="H14" s="17">
-        <f>Sheet1!B$29/ICStoDCP!B14</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="I14" s="17">
-        <f>Sheet1!C$29/ICStoDCP!C14</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="J14" s="17">
-        <f>Sheet1!D$29/ICStoDCP!D14</f>
-        <v>10</v>
-      </c>
-      <c r="K14" s="16">
-        <f>Sheet1!B$27/ICStoDCP!B14</f>
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="L14" s="16">
-        <f>Sheet1!C$27/ICStoDCP!C14</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="M14" s="16">
-        <f>Sheet1!D$27/ICStoDCP!D14</f>
-        <v>4.166666666666667</v>
+      <c r="H14" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I14" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J14" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K14" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L14" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M14" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D14</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix ICS folder for new ICS excel file and plots
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63C8CFF-592F-43FD-B532-430076367862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E534AC-F597-4CFE-A36F-BBFB945F4DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-2640" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Capacities" sheetId="5" r:id="rId2"/>
-    <sheet name="ICStoDCP" sheetId="3" r:id="rId3"/>
-    <sheet name="DCPLogs" sheetId="4" r:id="rId4"/>
-    <sheet name="By User" sheetId="2" r:id="rId5"/>
+    <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
+    <sheet name="Balances" sheetId="1" r:id="rId2"/>
+    <sheet name="Capacities" sheetId="5" r:id="rId3"/>
+    <sheet name="ICStoDCP" sheetId="3" r:id="rId4"/>
+    <sheet name="DCPLogs" sheetId="4" r:id="rId5"/>
+    <sheet name="By User" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="77">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -87,9 +88,6 @@
     <t>Balance - Dec 2015 (AF)</t>
   </si>
   <si>
-    <t>Intentionally Created Surplus (Lake Mead) - Summary Accounting</t>
-  </si>
-  <si>
     <t>Assessment of Losses</t>
   </si>
   <si>
@@ -186,15 +184,6 @@
     <t>NV</t>
   </si>
   <si>
-    <t>Percent of DCP obligation ICS max withdrawal can meet</t>
-  </si>
-  <si>
-    <t>Percent of DCP obliation max ICS deposit can fund</t>
-  </si>
-  <si>
-    <t>Annual Addition</t>
-  </si>
-  <si>
     <t>Balance - Dec 2020 (AF)</t>
   </si>
   <si>
@@ -244,6 +233,45 @@
   </si>
   <si>
     <t>Balance - Dec 2007 (AF)</t>
+  </si>
+  <si>
+    <t>Lake Mead Water Conservation Accounts (Intentionally Created Surplus) Data</t>
+  </si>
+  <si>
+    <t>Worksheet</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>1. Balances</t>
+  </si>
+  <si>
+    <t>Water Conservation account balances, credits, and debits, by year and entity.</t>
+  </si>
+  <si>
+    <t>2. Capacities</t>
+  </si>
+  <si>
+    <t>Maximum credits, debits, and totals allowed per year</t>
+  </si>
+  <si>
+    <t>3. ICStoDPC</t>
+  </si>
+  <si>
+    <t>4. DCPLogs</t>
+  </si>
+  <si>
+    <t>5. ByUser</t>
+  </si>
+  <si>
+    <t>Account balance by contractor</t>
+  </si>
+  <si>
+    <t>Explanation of how users met drought contingency plan (DPC) required conservation.</t>
+  </si>
+  <si>
+    <t>Number of years state can use ICS balance to meet drought contingency plan (DCP) required conservation</t>
   </si>
 </sst>
 </file>
@@ -279,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +323,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,12 +366,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -370,10 +403,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,17 +416,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -674,14 +700,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049640DB-DC1D-4720-8967-8C163BD4DD2C}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="46.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10:L23"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,864 +813,833 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="B2" s="3">
+        <v>710589</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1661832</v>
+      </c>
+      <c r="D2" s="3">
+        <v>955543</v>
+      </c>
+      <c r="E2" s="19">
+        <f>E3-34000</f>
+        <v>210975</v>
+      </c>
+      <c r="F2" s="2">
+        <f t="shared" ref="F2:F4" si="0">SUM(B2:D2)</f>
+        <v>3327964</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H2" s="11">
+        <f>F2-F3</f>
+        <v>290083</v>
+      </c>
+      <c r="I2" s="16">
+        <f t="shared" ref="I2" si="1">B2-B3</f>
+        <v>-42834</v>
+      </c>
+      <c r="J2" s="16">
+        <f t="shared" ref="J2" si="2">C2-C3</f>
+        <v>416139</v>
+      </c>
+      <c r="K2" s="16">
+        <f t="shared" ref="K2" si="3">D2-D3</f>
+        <v>-83222</v>
+      </c>
+      <c r="L2" s="16">
+        <f t="shared" ref="L2" si="4">E2-E3</f>
+        <v>-34000</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="12">
+        <v>753423</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1245693</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1038765</v>
+      </c>
+      <c r="E3" s="17">
+        <f>30000+E4</f>
+        <v>244975</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" si="0"/>
+        <v>3037881</v>
+      </c>
+      <c r="G3" s="18">
+        <v>2022</v>
+      </c>
+      <c r="H3" s="11">
+        <f>F3-F4</f>
+        <v>46937</v>
+      </c>
+      <c r="I3" s="16">
+        <f t="shared" ref="I3:I4" si="5">B3-B4</f>
+        <v>69222</v>
+      </c>
+      <c r="J3" s="16">
+        <f t="shared" ref="J3:J4" si="6">C3-C4</f>
+        <v>-111392</v>
+      </c>
+      <c r="K3" s="16">
+        <f t="shared" ref="K3:K4" si="7">D3-D4</f>
+        <v>89107</v>
+      </c>
+      <c r="L3" s="16">
+        <f t="shared" ref="L3:L4" si="8">E3-E4</f>
+        <v>30000</v>
+      </c>
+      <c r="N3" s="11">
+        <f t="shared" ref="N3:N4" si="9">SUM(E3:F3)</f>
+        <v>3282856</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="12">
+        <v>684201</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1357085</v>
+      </c>
+      <c r="D4" s="12">
+        <v>949658</v>
+      </c>
+      <c r="E4" s="17">
+        <f>41000+E5</f>
+        <v>214975</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>2990944</v>
+      </c>
+      <c r="G4" s="18">
+        <v>2021</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" ref="H4" si="10">F4-F5</f>
+        <v>150590</v>
+      </c>
+      <c r="I4" s="16">
+        <f t="shared" si="5"/>
+        <v>85459</v>
+      </c>
+      <c r="J4" s="16">
+        <f t="shared" si="6"/>
+        <v>-18786</v>
+      </c>
+      <c r="K4" s="16">
+        <f t="shared" si="7"/>
+        <v>83917</v>
+      </c>
+      <c r="L4" s="16">
+        <f t="shared" si="8"/>
+        <v>41000</v>
+      </c>
+      <c r="N4" s="11">
+        <f t="shared" si="9"/>
+        <v>3205919</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H5" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="17">
+        <v>598742</v>
+      </c>
+      <c r="C5" s="17">
+        <v>1375871</v>
+      </c>
+      <c r="D5" s="17">
+        <v>865741</v>
+      </c>
+      <c r="E5" s="17">
+        <f>41000+E6</f>
+        <v>173975</v>
+      </c>
+      <c r="F5" s="2">
+        <f>SUM(B5:D5)</f>
+        <v>2840354</v>
+      </c>
+      <c r="G5" s="18">
+        <v>2020</v>
+      </c>
+      <c r="H5" s="11">
+        <f>F5-F6</f>
+        <v>527727</v>
+      </c>
+      <c r="I5" s="16">
+        <f t="shared" ref="I5:L18" si="11">B5-B6</f>
+        <v>125238</v>
+      </c>
+      <c r="J5" s="16">
+        <f t="shared" si="11"/>
+        <v>322661</v>
+      </c>
+      <c r="K5" s="16">
+        <f t="shared" si="11"/>
+        <v>79828</v>
+      </c>
+      <c r="L5" s="16">
+        <f t="shared" si="11"/>
+        <v>41000</v>
+      </c>
+      <c r="N5" s="11">
+        <f>SUM(E5:F5)</f>
+        <v>3014329</v>
+      </c>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>61</v>
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>473504</v>
+      </c>
+      <c r="C6" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>1053210</v>
+      </c>
+      <c r="D6" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>785913</v>
+      </c>
+      <c r="E6" s="2">
+        <v>132975</v>
+      </c>
+      <c r="F6" s="2">
+        <f>SUM(B6:D6)</f>
+        <v>2312627</v>
+      </c>
+      <c r="G6" s="12">
+        <v>2019</v>
+      </c>
+      <c r="H6" s="11">
+        <f>F6-F7</f>
+        <v>570695</v>
+      </c>
+      <c r="I6" s="16">
+        <f t="shared" si="11"/>
+        <v>130452</v>
+      </c>
+      <c r="J6" s="16">
+        <f t="shared" si="11"/>
+        <v>354778</v>
+      </c>
+      <c r="K6" s="16">
+        <f t="shared" si="11"/>
+        <v>85465</v>
+      </c>
+      <c r="L6" s="16">
+        <f t="shared" si="11"/>
+        <v>132975</v>
+      </c>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16">
+        <f>H6-H5</f>
+        <v>42968</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="3">
-        <v>710589</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1661832</v>
-      </c>
-      <c r="D7" s="3">
-        <v>955543</v>
-      </c>
-      <c r="E7" s="21">
-        <f>E8-34000</f>
-        <v>210975</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B7" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>343052</v>
+      </c>
+      <c r="C7" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>698432</v>
+      </c>
+      <c r="D7" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>700448</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2">
-        <f t="shared" ref="F7:F9" si="0">SUM(B7:D7)</f>
-        <v>3327964</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2023</v>
+        <f>SUM(B7:D7)</f>
+        <v>1741932</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2018</v>
       </c>
       <c r="H7" s="11">
         <f>F7-F8</f>
-        <v>290083</v>
-      </c>
-      <c r="I7" s="18">
-        <f t="shared" ref="I7" si="1">B7-B8</f>
-        <v>-42834</v>
-      </c>
-      <c r="J7" s="18">
-        <f t="shared" ref="J7" si="2">C7-C8</f>
-        <v>416139</v>
-      </c>
-      <c r="K7" s="18">
-        <f t="shared" ref="K7" si="3">D7-D8</f>
-        <v>-83222</v>
-      </c>
-      <c r="L7" s="18">
-        <f t="shared" ref="L7" si="4">E7-E8</f>
-        <v>-34000</v>
+        <v>480441</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" ref="I7:I14" si="12">B7-B8</f>
+        <v>216252</v>
+      </c>
+      <c r="J7" s="16">
+        <f t="shared" ref="J7:J14" si="13">C7-C8</f>
+        <v>146054</v>
+      </c>
+      <c r="K7" s="16">
+        <f t="shared" ref="K7:K14" si="14">D7-D8</f>
+        <v>118135</v>
+      </c>
+      <c r="L7" s="16">
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="12">
-        <v>753423</v>
-      </c>
-      <c r="C8" s="12">
-        <v>1245693</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1038765</v>
-      </c>
-      <c r="E8" s="19">
-        <f>30000+E9</f>
-        <v>244975</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>126800</v>
+      </c>
+      <c r="C8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>552378</v>
+      </c>
+      <c r="D8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>582313</v>
+      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>3037881</v>
-      </c>
-      <c r="G8" s="20">
-        <v>2022</v>
+        <f>SUM(B8:D8)</f>
+        <v>1261491</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2017</v>
       </c>
       <c r="H8" s="11">
-        <f>F8-F9</f>
-        <v>46937</v>
-      </c>
-      <c r="I8" s="18">
-        <f t="shared" ref="I8:I9" si="5">B8-B9</f>
-        <v>69222</v>
-      </c>
-      <c r="J8" s="18">
-        <f t="shared" ref="J8:J9" si="6">C8-C9</f>
-        <v>-111392</v>
-      </c>
-      <c r="K8" s="18">
-        <f t="shared" ref="K8:K9" si="7">D8-D9</f>
-        <v>89107</v>
-      </c>
-      <c r="L8" s="18">
-        <f t="shared" ref="L8:L9" si="8">E8-E9</f>
-        <v>30000</v>
-      </c>
-      <c r="N8" s="11">
-        <f t="shared" ref="N8:N9" si="9">SUM(E8:F8)</f>
-        <v>3282856</v>
+        <f t="shared" ref="H8:H14" si="15">F8-F9</f>
+        <v>511813</v>
+      </c>
+      <c r="I8" s="16">
+        <f t="shared" si="12"/>
+        <v>23750</v>
+      </c>
+      <c r="J8" s="16">
+        <f t="shared" si="13"/>
+        <v>437312</v>
+      </c>
+      <c r="K8" s="16">
+        <f t="shared" si="14"/>
+        <v>50751</v>
+      </c>
+      <c r="L8" s="16">
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="12">
-        <v>684201</v>
-      </c>
-      <c r="C9" s="12">
-        <v>1357085</v>
-      </c>
-      <c r="D9" s="12">
-        <v>949658</v>
-      </c>
-      <c r="E9" s="19">
-        <f>41000+E10</f>
-        <v>214975</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
+      </c>
+      <c r="C9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>115066</v>
+      </c>
+      <c r="D9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>531562</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>2990944</v>
-      </c>
-      <c r="G9" s="20">
-        <v>2021</v>
+        <f t="shared" ref="F9:F18" si="16">SUM(B9:D9)</f>
+        <v>749678</v>
+      </c>
+      <c r="G9" s="10">
+        <v>2016</v>
       </c>
       <c r="H9" s="11">
-        <f t="shared" ref="H9" si="10">F9-F10</f>
-        <v>150590</v>
-      </c>
-      <c r="I9" s="18">
-        <f t="shared" si="5"/>
-        <v>85459</v>
-      </c>
-      <c r="J9" s="18">
-        <f t="shared" si="6"/>
-        <v>-18786</v>
-      </c>
-      <c r="K9" s="18">
-        <f t="shared" si="7"/>
-        <v>83917</v>
-      </c>
-      <c r="L9" s="18">
-        <f t="shared" si="8"/>
-        <v>41000</v>
-      </c>
-      <c r="N9" s="11">
-        <f t="shared" si="9"/>
-        <v>3205919</v>
+        <f t="shared" si="15"/>
+        <v>37814</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="16">
+        <f t="shared" si="13"/>
+        <v>17275</v>
+      </c>
+      <c r="K9" s="16">
+        <f t="shared" si="14"/>
+        <v>20539</v>
+      </c>
+      <c r="L9" s="16">
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="19">
-        <v>598742</v>
-      </c>
-      <c r="C10" s="19">
-        <v>1375871</v>
-      </c>
-      <c r="D10" s="19">
-        <v>865741</v>
-      </c>
-      <c r="E10" s="19">
-        <f>41000+E11</f>
-        <v>173975</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G10,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
+      </c>
+      <c r="C10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G10,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>97791</v>
+      </c>
+      <c r="D10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G10,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>511023</v>
+      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2">
-        <f>SUM(B10:D10)</f>
-        <v>2840354</v>
-      </c>
-      <c r="G10" s="20">
-        <v>2020</v>
+        <f t="shared" si="16"/>
+        <v>711864</v>
+      </c>
+      <c r="G10" s="10">
+        <v>2015</v>
       </c>
       <c r="H10" s="11">
-        <f>F10-F11</f>
-        <v>527727</v>
-      </c>
-      <c r="I10" s="18">
-        <f t="shared" ref="I10:L23" si="11">B10-B11</f>
-        <v>125238</v>
-      </c>
-      <c r="J10" s="18">
+        <f t="shared" si="15"/>
+        <v>-125036</v>
+      </c>
+      <c r="I10" s="16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="16">
+        <f t="shared" si="13"/>
+        <v>-71294</v>
+      </c>
+      <c r="K10" s="16">
+        <f t="shared" si="14"/>
+        <v>-53742</v>
+      </c>
+      <c r="L10" s="16">
         <f t="shared" si="11"/>
-        <v>322661</v>
-      </c>
-      <c r="K10" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
+      </c>
+      <c r="C11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>169085</v>
+      </c>
+      <c r="D11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>564765</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
+        <f t="shared" si="16"/>
+        <v>836900</v>
+      </c>
+      <c r="G11" s="10">
+        <v>2014</v>
+      </c>
+      <c r="H11" s="11">
+        <f t="shared" si="15"/>
+        <v>-281264</v>
+      </c>
+      <c r="I11" s="16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="16">
+        <f t="shared" si="13"/>
+        <v>-304978</v>
+      </c>
+      <c r="K11" s="16">
+        <f t="shared" si="14"/>
+        <v>23714</v>
+      </c>
+      <c r="L11" s="16">
         <f t="shared" si="11"/>
-        <v>79828</v>
-      </c>
-      <c r="L10" s="18">
-        <f t="shared" si="11"/>
-        <v>41000</v>
-      </c>
-      <c r="N10" s="11">
-        <f>SUM(E10:F10)</f>
-        <v>3014329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>473504</v>
-      </c>
-      <c r="C11" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>1053210</v>
-      </c>
-      <c r="D11" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>785913</v>
-      </c>
-      <c r="E11" s="2">
-        <v>132975</v>
-      </c>
-      <c r="F11" s="2">
-        <f>SUM(B11:D11)</f>
-        <v>2312627</v>
-      </c>
-      <c r="G11" s="12">
-        <v>2019</v>
-      </c>
-      <c r="H11" s="11">
-        <f>F11-F12</f>
-        <v>570695</v>
-      </c>
-      <c r="I11" s="18">
-        <f t="shared" si="11"/>
-        <v>130452</v>
-      </c>
-      <c r="J11" s="18">
-        <f t="shared" si="11"/>
-        <v>354778</v>
-      </c>
-      <c r="K11" s="18">
-        <f t="shared" si="11"/>
-        <v>85465</v>
-      </c>
-      <c r="L11" s="18">
-        <f t="shared" si="11"/>
-        <v>132975</v>
-      </c>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18">
-        <f>H11-H10</f>
-        <v>42968</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>343052</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
       </c>
       <c r="C12" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>698432</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>474063</v>
       </c>
       <c r="D12" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>700448</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>541051</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
-        <f>SUM(B12:D12)</f>
-        <v>1741932</v>
-      </c>
-      <c r="G12" s="9">
-        <v>2018</v>
+        <f t="shared" si="16"/>
+        <v>1118164</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2013</v>
       </c>
       <c r="H12" s="11">
-        <f>F12-F13</f>
-        <v>480441</v>
-      </c>
-      <c r="I12" s="18">
-        <f t="shared" ref="I12:I19" si="12">B12-B13</f>
-        <v>216252</v>
-      </c>
-      <c r="J12" s="18">
-        <f t="shared" ref="J12:J19" si="13">C12-C13</f>
-        <v>146054</v>
-      </c>
-      <c r="K12" s="18">
-        <f t="shared" ref="K12:K19" si="14">D12-D13</f>
-        <v>118135</v>
-      </c>
-      <c r="L12" s="18">
+        <f t="shared" si="15"/>
+        <v>-77476</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="16">
+        <f t="shared" si="13"/>
+        <v>-105723</v>
+      </c>
+      <c r="K12" s="16">
+        <f t="shared" si="14"/>
+        <v>28247</v>
+      </c>
+      <c r="L12" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>126800</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
       </c>
       <c r="C13" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>552378</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>579786</v>
       </c>
       <c r="D13" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>582313</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>512804</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
-        <f>SUM(B13:D13)</f>
-        <v>1261491</v>
+        <f t="shared" si="16"/>
+        <v>1195640</v>
       </c>
       <c r="G13" s="10">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="H13" s="11">
-        <f t="shared" ref="H13:H19" si="15">F13-F14</f>
-        <v>511813</v>
-      </c>
-      <c r="I13" s="18">
+        <f t="shared" si="15"/>
+        <v>169240</v>
+      </c>
+      <c r="I13" s="16">
         <f t="shared" si="12"/>
-        <v>23750</v>
-      </c>
-      <c r="J13" s="18">
+        <v>0</v>
+      </c>
+      <c r="J13" s="16">
         <f t="shared" si="13"/>
-        <v>437312</v>
-      </c>
-      <c r="K13" s="18">
+        <v>139108</v>
+      </c>
+      <c r="K13" s="16">
         <f t="shared" si="14"/>
-        <v>50751</v>
-      </c>
-      <c r="L13" s="18">
+        <v>30132</v>
+      </c>
+      <c r="L13" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!B$1)</f>
         <v>103050</v>
       </c>
       <c r="C14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>115066</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>440678</v>
       </c>
       <c r="D14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>531562</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>482672</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
-        <f t="shared" ref="F14:F23" si="16">SUM(B14:D14)</f>
-        <v>749678</v>
+        <f t="shared" si="16"/>
+        <v>1026400</v>
       </c>
       <c r="G14" s="10">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="H14" s="11">
         <f t="shared" si="15"/>
-        <v>37814</v>
-      </c>
-      <c r="I14" s="18">
+        <v>211059</v>
+      </c>
+      <c r="I14" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="18">
+        <v>956</v>
+      </c>
+      <c r="J14" s="16">
         <f t="shared" si="13"/>
-        <v>17275</v>
-      </c>
-      <c r="K14" s="18">
+        <v>178688</v>
+      </c>
+      <c r="K14" s="16">
         <f t="shared" si="14"/>
-        <v>20539</v>
-      </c>
-      <c r="L14" s="18">
+        <v>31415</v>
+      </c>
+      <c r="L14" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G15,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>102094</v>
       </c>
       <c r="C15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>97791</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G15,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>261990</v>
       </c>
       <c r="D15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>511023</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G15,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>451257</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
         <f t="shared" si="16"/>
-        <v>711864</v>
+        <v>815341</v>
       </c>
       <c r="G15" s="10">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="H15" s="11">
-        <f t="shared" si="15"/>
-        <v>-125036</v>
-      </c>
-      <c r="I15" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="18">
-        <f t="shared" si="13"/>
-        <v>-71294</v>
-      </c>
-      <c r="K15" s="18">
-        <f t="shared" si="14"/>
-        <v>-53742</v>
-      </c>
-      <c r="L15" s="18">
+        <f t="shared" ref="H15:H18" si="17">F15-F16</f>
+        <v>158151</v>
+      </c>
+      <c r="I15" s="16">
+        <f t="shared" ref="I15:I18" si="18">B15-B16</f>
+        <v>2094</v>
+      </c>
+      <c r="J15" s="16">
+        <f t="shared" ref="J15:J18" si="19">C15-C16</f>
+        <v>104800</v>
+      </c>
+      <c r="K15" s="16">
+        <f t="shared" ref="K15:K18" si="20">D15-D16</f>
+        <v>51257</v>
+      </c>
+      <c r="L15" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <v>100000</v>
       </c>
       <c r="C16" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>169085</v>
+        <f>79790+66000+11400</f>
+        <v>157190</v>
       </c>
       <c r="D16" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>564765</v>
+        <v>400000</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2">
         <f t="shared" si="16"/>
-        <v>836900</v>
+        <v>657190</v>
       </c>
       <c r="G16" s="10">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="H16" s="11">
-        <f t="shared" si="15"/>
-        <v>-281264</v>
-      </c>
-      <c r="I16" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="18">
-        <f t="shared" si="13"/>
-        <v>-304978</v>
-      </c>
-      <c r="K16" s="18">
-        <f t="shared" si="14"/>
-        <v>23714</v>
-      </c>
-      <c r="L16" s="18">
+        <f t="shared" si="17"/>
+        <v>63617</v>
+      </c>
+      <c r="I16" s="16">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="16">
+        <f t="shared" si="19"/>
+        <v>63617</v>
+      </c>
+      <c r="K16" s="16">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="B17" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <v>100000</v>
       </c>
       <c r="C17" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>474063</v>
+        <f>27573+66000</f>
+        <v>93573</v>
       </c>
       <c r="D17" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>541051</v>
+        <v>400000</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2">
         <f t="shared" si="16"/>
-        <v>1118164</v>
+        <v>593573</v>
       </c>
       <c r="G17" s="10">
-        <v>2013</v>
+        <v>2008</v>
       </c>
       <c r="H17" s="11">
-        <f t="shared" si="15"/>
-        <v>-77476</v>
-      </c>
-      <c r="I17" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="18">
-        <f t="shared" si="13"/>
-        <v>-105723</v>
-      </c>
-      <c r="K17" s="18">
-        <f t="shared" si="14"/>
-        <v>28247</v>
-      </c>
-      <c r="L17" s="18">
+        <f t="shared" si="17"/>
+        <v>552175</v>
+      </c>
+      <c r="I17" s="16">
+        <f t="shared" si="18"/>
+        <v>100000</v>
+      </c>
+      <c r="J17" s="16">
+        <f t="shared" si="19"/>
+        <v>52175</v>
+      </c>
+      <c r="K17" s="16">
+        <f t="shared" si="20"/>
+        <v>400000</v>
+      </c>
+      <c r="L17" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="B18" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>579786</v>
+        <v>41398</v>
       </c>
       <c r="D18" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>512804</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2">
         <f t="shared" si="16"/>
-        <v>1195640</v>
+        <v>41398</v>
       </c>
       <c r="G18" s="10">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="H18" s="11">
-        <f t="shared" si="15"/>
-        <v>169240</v>
-      </c>
-      <c r="I18" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="18">
-        <f t="shared" si="13"/>
-        <v>139108</v>
-      </c>
-      <c r="K18" s="18">
-        <f t="shared" si="14"/>
-        <v>30132</v>
-      </c>
-      <c r="L18" s="18">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
-      </c>
-      <c r="C19" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>440678</v>
-      </c>
-      <c r="D19" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>482672</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2">
-        <f t="shared" si="16"/>
-        <v>1026400</v>
-      </c>
-      <c r="G19" s="10">
-        <v>2011</v>
-      </c>
-      <c r="H19" s="11">
-        <f t="shared" si="15"/>
-        <v>211059</v>
-      </c>
-      <c r="I19" s="18">
-        <f t="shared" si="12"/>
-        <v>956</v>
-      </c>
-      <c r="J19" s="18">
-        <f t="shared" si="13"/>
-        <v>178688</v>
-      </c>
-      <c r="K19" s="18">
-        <f t="shared" si="14"/>
-        <v>31415</v>
-      </c>
-      <c r="L19" s="18">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>102094</v>
-      </c>
-      <c r="C20" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>261990</v>
-      </c>
-      <c r="D20" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>451257</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2">
-        <f t="shared" si="16"/>
-        <v>815341</v>
-      </c>
-      <c r="G20" s="10">
-        <v>2010</v>
-      </c>
-      <c r="H20" s="11">
-        <f t="shared" ref="H20:H23" si="17">F20-F21</f>
-        <v>158151</v>
-      </c>
-      <c r="I20" s="18">
-        <f t="shared" ref="I20:I23" si="18">B20-B21</f>
-        <v>2094</v>
-      </c>
-      <c r="J20" s="18">
-        <f t="shared" ref="J20:J23" si="19">C20-C21</f>
-        <v>104800</v>
-      </c>
-      <c r="K20" s="18">
-        <f t="shared" ref="K20:K23" si="20">D20-D21</f>
-        <v>51257</v>
-      </c>
-      <c r="L20" s="18">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="2">
-        <v>100000</v>
-      </c>
-      <c r="C21" s="2">
-        <f>79790+66000+11400</f>
-        <v>157190</v>
-      </c>
-      <c r="D21" s="2">
-        <v>400000</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2">
-        <f t="shared" si="16"/>
-        <v>657190</v>
-      </c>
-      <c r="G21" s="10">
-        <v>2009</v>
-      </c>
-      <c r="H21" s="11">
-        <f t="shared" si="17"/>
-        <v>63617</v>
-      </c>
-      <c r="I21" s="18">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="18">
-        <f t="shared" si="19"/>
-        <v>63617</v>
-      </c>
-      <c r="K21" s="18">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="18">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="2">
-        <v>100000</v>
-      </c>
-      <c r="C22" s="2">
-        <f>27573+66000</f>
-        <v>93573</v>
-      </c>
-      <c r="D22" s="2">
-        <v>400000</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2">
-        <f t="shared" si="16"/>
-        <v>593573</v>
-      </c>
-      <c r="G22" s="10">
-        <v>2008</v>
-      </c>
-      <c r="H22" s="11">
-        <f t="shared" si="17"/>
-        <v>552175</v>
-      </c>
-      <c r="I22" s="18">
-        <f t="shared" si="18"/>
-        <v>100000</v>
-      </c>
-      <c r="J22" s="18">
-        <f t="shared" si="19"/>
-        <v>52175</v>
-      </c>
-      <c r="K22" s="18">
-        <f t="shared" si="20"/>
-        <v>400000</v>
-      </c>
-      <c r="L22" s="18">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="2">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
-        <v>41398</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2">
-        <f t="shared" si="16"/>
-        <v>41398</v>
-      </c>
-      <c r="G23" s="10">
-        <v>2007</v>
-      </c>
-      <c r="H23" s="11">
         <f t="shared" si="17"/>
         <v>41398</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I18" s="16">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="J23" s="18">
+      <c r="J18" s="16">
         <f t="shared" si="19"/>
         <v>41398</v>
       </c>
-      <c r="K23" s="18">
+      <c r="K18" s="16">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="L23" s="18">
+      <c r="L18" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H5:K5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9C09D6-2BEE-4EAC-9C47-48919B4DAC3E}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1580,7 +1663,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -1645,7 +1728,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1662,7 +1745,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="8" t="str">
         <f>B1</f>
@@ -1706,7 +1789,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="6">
         <v>500000</v>
@@ -1746,18 +1829,18 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="A11" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1774,7 +1857,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1794,7 +1877,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="4">
         <v>0.03</v>
@@ -1815,12 +1898,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H1" sqref="H1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1830,61 +1913,37 @@
     <col min="4" max="4" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E1" s="24" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="14">
         <v>1218.5</v>
       </c>
@@ -1892,7 +1951,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="14">
         <v>1190</v>
       </c>
@@ -1900,7 +1959,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="14">
         <v>1150</v>
       </c>
@@ -1908,7 +1967,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>1091</v>
       </c>
@@ -1916,7 +1975,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>1090</v>
       </c>
@@ -1928,34 +1987,16 @@
         <v>8000</v>
       </c>
       <c r="E7" s="15">
-        <f>Sheet1!B$10/B7</f>
+        <f>Balances!B$5/B7</f>
         <v>3.1184479166666668</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15">
-        <f>Sheet1!D$10/D7</f>
+        <f>Balances!D$5/D7</f>
         <v>108.217625</v>
       </c>
-      <c r="H7" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B7</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D7</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K7" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B7</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D7</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>1075</v>
       </c>
@@ -1967,34 +2008,16 @@
         <v>21000</v>
       </c>
       <c r="E8" s="15">
-        <f>Sheet1!B$10/B8</f>
+        <f>Balances!B$5/B8</f>
         <v>1.1694179687499999</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15">
-        <f>Sheet1!D$10/D8</f>
+        <f>Balances!D$5/D8</f>
         <v>41.225761904761903</v>
       </c>
-      <c r="H8" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K8" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D8</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>1050</v>
       </c>
@@ -2006,34 +2029,16 @@
         <v>25000</v>
       </c>
       <c r="E9" s="15">
-        <f>Sheet1!B$10/B9</f>
+        <f>Balances!B$5/B9</f>
         <v>1.0113885135135134</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15">
-        <f>Sheet1!D$10/D9</f>
+        <f>Balances!D$5/D9</f>
         <v>34.629640000000002</v>
       </c>
-      <c r="H9" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K9" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D9</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>1045</v>
       </c>
@@ -2047,43 +2052,19 @@
         <v>27000</v>
       </c>
       <c r="E10" s="15">
-        <f>Sheet1!B$10/B10</f>
+        <f>Balances!B$5/B10</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F10" s="15">
-        <f>Sheet1!C$10/C10</f>
+        <f>Balances!C$5/C10</f>
         <v>6.8793550000000003</v>
       </c>
       <c r="G10" s="15">
-        <f>Sheet1!D$10/D10</f>
+        <f>Balances!D$5/D10</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H10" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I10" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J10" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K10" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L10" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M10" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D10</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>1040</v>
       </c>
@@ -2097,43 +2078,19 @@
         <v>27000</v>
       </c>
       <c r="E11" s="15">
-        <f>Sheet1!B$10/B11</f>
+        <f>Balances!B$5/B11</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F11" s="15">
-        <f>Sheet1!C$10/C11</f>
+        <f>Balances!C$5/C11</f>
         <v>5.5034840000000003</v>
       </c>
       <c r="G11" s="15">
-        <f>Sheet1!D$10/D11</f>
+        <f>Balances!D$5/D11</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H11" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I11" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J11" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K11" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L11" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M11" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D11</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>1035</v>
       </c>
@@ -2147,43 +2104,19 @@
         <v>27000</v>
       </c>
       <c r="E12" s="15">
-        <f>Sheet1!B$10/B12</f>
+        <f>Balances!B$5/B12</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F12" s="15">
-        <f>Sheet1!C$10/C12</f>
+        <f>Balances!C$5/C12</f>
         <v>4.5862366666666663</v>
       </c>
       <c r="G12" s="15">
-        <f>Sheet1!D$10/D12</f>
+        <f>Balances!D$5/D12</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H12" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I12" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J12" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K12" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L12" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M12" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D12</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>1030</v>
       </c>
@@ -2197,43 +2130,19 @@
         <v>27000</v>
       </c>
       <c r="E13" s="15">
-        <f>Sheet1!B$10/B13</f>
+        <f>Balances!B$5/B13</f>
         <v>0.93553437500000003</v>
       </c>
       <c r="F13" s="15">
-        <f>Sheet1!C$10/C13</f>
+        <f>Balances!C$5/C13</f>
         <v>3.93106</v>
       </c>
       <c r="G13" s="15">
-        <f>Sheet1!D$10/D13</f>
+        <f>Balances!D$5/D13</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H13" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I13" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K13" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L13" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M13" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D13</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>1025</v>
       </c>
@@ -2247,40 +2156,16 @@
         <v>30000</v>
       </c>
       <c r="E14" s="15">
-        <f>Sheet1!B$10/B14</f>
+        <f>Balances!B$5/B14</f>
         <v>0.83158611111111114</v>
       </c>
       <c r="F14" s="15">
-        <f>Sheet1!C$10/C14</f>
+        <f>Balances!C$5/C14</f>
         <v>3.93106</v>
       </c>
       <c r="G14" s="15">
-        <f>Sheet1!D$10/D14</f>
+        <f>Balances!D$5/D14</f>
         <v>28.858033333333335</v>
-      </c>
-      <c r="H14" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I14" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J14" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K14" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L14" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M14" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D14</f>
-        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -2291,7 +2176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
   <dimension ref="A2:I7"/>
   <sheetViews>
@@ -2310,31 +2195,31 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>55</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2342,7 +2227,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>2020</v>
@@ -2399,7 +2284,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>2020</v>
@@ -2434,11 +2319,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A42" sqref="A42:D42"/>
     </sheetView>
   </sheetViews>
@@ -2450,16 +2335,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -2467,7 +2352,7 @@
         <v>2011</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -2484,7 +2369,7 @@
         <v>2011</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -2499,7 +2384,7 @@
         <v>2011</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -2514,7 +2399,7 @@
         <v>2011</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -2529,7 +2414,7 @@
         <v>2010</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -2544,7 +2429,7 @@
         <v>2010</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2559,7 +2444,7 @@
         <v>2010</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -2573,7 +2458,7 @@
         <v>2010</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -2589,7 +2474,7 @@
         <v>2012</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -2604,7 +2489,7 @@
         <v>2012</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -2619,7 +2504,7 @@
         <v>2012</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -2633,7 +2518,7 @@
         <v>2012</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -2649,7 +2534,7 @@
         <v>2013</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -2664,7 +2549,7 @@
         <v>2013</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -2679,7 +2564,7 @@
         <v>2013</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -2693,7 +2578,7 @@
         <v>2013</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -2708,7 +2593,7 @@
         <v>2014</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -2723,7 +2608,7 @@
         <v>2014</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2738,7 +2623,7 @@
         <v>2014</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -2752,7 +2637,7 @@
         <v>2014</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2766,7 +2651,7 @@
         <v>2015</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -2781,7 +2666,7 @@
         <v>2015</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -2796,7 +2681,7 @@
         <v>2015</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2810,7 +2695,7 @@
         <v>2015</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -2824,7 +2709,7 @@
         <v>2016</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -2839,7 +2724,7 @@
         <v>2016</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -2854,7 +2739,7 @@
         <v>2016</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -2868,7 +2753,7 @@
         <v>2016</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -2882,7 +2767,7 @@
         <v>2017</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -2896,7 +2781,7 @@
         <v>2017</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -2910,7 +2795,7 @@
         <v>2017</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -2924,7 +2809,7 @@
         <v>2017</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -2938,7 +2823,7 @@
         <v>2018</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -2952,7 +2837,7 @@
         <v>2018</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -2966,7 +2851,7 @@
         <v>2018</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -2980,7 +2865,7 @@
         <v>2018</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -2994,7 +2879,7 @@
         <v>2019</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
         <v>3</v>
@@ -3008,7 +2893,7 @@
         <v>2019</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
@@ -3022,7 +2907,7 @@
         <v>2019</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
@@ -3036,7 +2921,7 @@
         <v>2019</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -3050,7 +2935,7 @@
         <v>2019</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -3064,7 +2949,7 @@
         <v>2019</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update ICS Excel file to make from 2007 to 2023, move deposits to a separate worksheet. Propogate code in R file
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E534AC-F597-4CFE-A36F-BBFB945F4DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B7E62C-357D-49C9-BF3C-523C1106752D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
     <sheet name="Balances" sheetId="1" r:id="rId2"/>
-    <sheet name="Capacities" sheetId="5" r:id="rId3"/>
-    <sheet name="ICStoDCP" sheetId="3" r:id="rId4"/>
-    <sheet name="DCPLogs" sheetId="4" r:id="rId5"/>
-    <sheet name="By User" sheetId="2" r:id="rId6"/>
+    <sheet name="Deposits" sheetId="7" r:id="rId3"/>
+    <sheet name="Capacities" sheetId="5" r:id="rId4"/>
+    <sheet name="ICStoDCP" sheetId="3" r:id="rId5"/>
+    <sheet name="DCPLogs" sheetId="4" r:id="rId6"/>
+    <sheet name="By User" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -190,9 +213,6 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>MX</t>
-  </si>
-  <si>
     <t>Required DCP Contribution</t>
   </si>
   <si>
@@ -250,28 +270,34 @@
     <t>Water Conservation account balances, credits, and debits, by year and entity.</t>
   </si>
   <si>
-    <t>2. Capacities</t>
-  </si>
-  <si>
     <t>Maximum credits, debits, and totals allowed per year</t>
   </si>
   <si>
-    <t>3. ICStoDPC</t>
-  </si>
-  <si>
-    <t>4. DCPLogs</t>
-  </si>
-  <si>
-    <t>5. ByUser</t>
-  </si>
-  <si>
-    <t>Account balance by contractor</t>
-  </si>
-  <si>
     <t>Explanation of how users met drought contingency plan (DPC) required conservation.</t>
   </si>
   <si>
     <t>Number of years state can use ICS balance to meet drought contingency plan (DCP) required conservation</t>
+  </si>
+  <si>
+    <t>2. Deposits</t>
+  </si>
+  <si>
+    <t>Annual deposits and withdraws calculated as the year to year difference in balances.</t>
+  </si>
+  <si>
+    <t>3. Capacities</t>
+  </si>
+  <si>
+    <t>4. ICStoDPC</t>
+  </si>
+  <si>
+    <t>5. DCPLogs</t>
+  </si>
+  <si>
+    <t>6. ByUser</t>
+  </si>
+  <si>
+    <t>Account balance by state and contractor</t>
   </si>
 </sst>
 </file>
@@ -370,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -403,7 +429,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,13 +438,19 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -701,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049640DB-DC1D-4720-8967-8C163BD4DD2C}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -715,7 +746,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -735,51 +766,59 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
         <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -789,13 +828,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -806,12 +845,10 @@
     <col min="4" max="5" width="10.54296875" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" customWidth="1"/>
     <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="14" max="14" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -833,362 +870,190 @@
       <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>41398</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <f t="shared" ref="F2:F18" si="0">SUM(B2:D2)</f>
+        <v>41398</v>
+      </c>
+      <c r="G2" s="10">
+        <v>2007</v>
+      </c>
+      <c r="H2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C3" s="2">
+        <f>27573+66000</f>
+        <v>93573</v>
+      </c>
+      <c r="D3" s="2">
+        <v>400000</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <f t="shared" si="0"/>
+        <v>593573</v>
+      </c>
+      <c r="G3" s="10">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="3">
-        <v>710589</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1661832</v>
-      </c>
-      <c r="D2" s="3">
-        <v>955543</v>
-      </c>
-      <c r="E2" s="19">
-        <f>E3-34000</f>
-        <v>210975</v>
-      </c>
-      <c r="F2" s="2">
-        <f t="shared" ref="F2:F4" si="0">SUM(B2:D2)</f>
-        <v>3327964</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2023</v>
-      </c>
-      <c r="H2" s="11">
-        <f>F2-F3</f>
-        <v>290083</v>
-      </c>
-      <c r="I2" s="16">
-        <f t="shared" ref="I2" si="1">B2-B3</f>
-        <v>-42834</v>
-      </c>
-      <c r="J2" s="16">
-        <f t="shared" ref="J2" si="2">C2-C3</f>
-        <v>416139</v>
-      </c>
-      <c r="K2" s="16">
-        <f t="shared" ref="K2" si="3">D2-D3</f>
-        <v>-83222</v>
-      </c>
-      <c r="L2" s="16">
-        <f t="shared" ref="L2" si="4">E2-E3</f>
-        <v>-34000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="12">
-        <v>753423</v>
-      </c>
-      <c r="C3" s="12">
-        <v>1245693</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1038765</v>
-      </c>
-      <c r="E3" s="17">
-        <f>30000+E4</f>
-        <v>244975</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" si="0"/>
-        <v>3037881</v>
-      </c>
-      <c r="G3" s="18">
-        <v>2022</v>
-      </c>
-      <c r="H3" s="11">
-        <f>F3-F4</f>
-        <v>46937</v>
-      </c>
-      <c r="I3" s="16">
-        <f t="shared" ref="I3:I4" si="5">B3-B4</f>
-        <v>69222</v>
-      </c>
-      <c r="J3" s="16">
-        <f t="shared" ref="J3:J4" si="6">C3-C4</f>
-        <v>-111392</v>
-      </c>
-      <c r="K3" s="16">
-        <f t="shared" ref="K3:K4" si="7">D3-D4</f>
-        <v>89107</v>
-      </c>
-      <c r="L3" s="16">
-        <f t="shared" ref="L3:L4" si="8">E3-E4</f>
-        <v>30000</v>
-      </c>
-      <c r="N3" s="11">
-        <f t="shared" ref="N3:N4" si="9">SUM(E3:F3)</f>
-        <v>3282856</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="12">
-        <v>684201</v>
-      </c>
-      <c r="C4" s="12">
-        <v>1357085</v>
-      </c>
-      <c r="D4" s="12">
-        <v>949658</v>
-      </c>
-      <c r="E4" s="17">
-        <f>41000+E5</f>
-        <v>214975</v>
-      </c>
+      <c r="B4" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C4" s="2">
+        <f>79790+66000+11400</f>
+        <v>157190</v>
+      </c>
+      <c r="D4" s="2">
+        <v>400000</v>
+      </c>
+      <c r="E4" s="2"/>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>2990944</v>
-      </c>
-      <c r="G4" s="18">
-        <v>2021</v>
-      </c>
-      <c r="H4" s="11">
-        <f t="shared" ref="H4" si="10">F4-F5</f>
-        <v>150590</v>
-      </c>
-      <c r="I4" s="16">
-        <f t="shared" si="5"/>
-        <v>85459</v>
-      </c>
-      <c r="J4" s="16">
-        <f t="shared" si="6"/>
-        <v>-18786</v>
-      </c>
-      <c r="K4" s="16">
-        <f t="shared" si="7"/>
-        <v>83917</v>
-      </c>
-      <c r="L4" s="16">
-        <f t="shared" si="8"/>
-        <v>41000</v>
-      </c>
-      <c r="N4" s="11">
-        <f t="shared" si="9"/>
-        <v>3205919</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+        <v>657190</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="17">
-        <v>598742</v>
-      </c>
-      <c r="C5" s="17">
-        <v>1375871</v>
-      </c>
-      <c r="D5" s="17">
-        <v>865741</v>
-      </c>
-      <c r="E5" s="17">
-        <f>41000+E6</f>
-        <v>173975</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B5" s="2">
+        <v>102094</v>
+      </c>
+      <c r="C5" s="2">
+        <v>261990</v>
+      </c>
+      <c r="D5" s="2">
+        <v>451257</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2">
-        <f>SUM(B5:D5)</f>
-        <v>2840354</v>
-      </c>
-      <c r="G5" s="18">
-        <v>2020</v>
-      </c>
-      <c r="H5" s="11">
-        <f>F5-F6</f>
-        <v>527727</v>
-      </c>
-      <c r="I5" s="16">
-        <f t="shared" ref="I5:L18" si="11">B5-B6</f>
-        <v>125238</v>
-      </c>
-      <c r="J5" s="16">
-        <f t="shared" si="11"/>
-        <v>322661</v>
-      </c>
-      <c r="K5" s="16">
-        <f t="shared" si="11"/>
-        <v>79828</v>
-      </c>
-      <c r="L5" s="16">
-        <f t="shared" si="11"/>
-        <v>41000</v>
-      </c>
-      <c r="N5" s="11">
-        <f>SUM(E5:F5)</f>
-        <v>3014329</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>815341</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!B$1)</f>
-        <v>473504</v>
+        <v>103050</v>
       </c>
       <c r="C6" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!C$1)</f>
-        <v>1053210</v>
+        <v>440678</v>
       </c>
       <c r="D6" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!D$1)</f>
-        <v>785913</v>
+        <v>482672</v>
       </c>
       <c r="E6" s="2">
-        <v>132975</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
       </c>
       <c r="F6" s="2">
-        <f>SUM(B6:D6)</f>
-        <v>2312627</v>
-      </c>
-      <c r="G6" s="12">
-        <v>2019</v>
-      </c>
-      <c r="H6" s="11">
-        <f>F6-F7</f>
-        <v>570695</v>
-      </c>
-      <c r="I6" s="16">
-        <f t="shared" si="11"/>
-        <v>130452</v>
-      </c>
-      <c r="J6" s="16">
-        <f t="shared" si="11"/>
-        <v>354778</v>
-      </c>
-      <c r="K6" s="16">
-        <f t="shared" si="11"/>
-        <v>85465</v>
-      </c>
-      <c r="L6" s="16">
-        <f t="shared" si="11"/>
-        <v>132975</v>
-      </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16">
-        <f>H6-H5</f>
-        <v>42968</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1026400</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2011</v>
+      </c>
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!B$1)</f>
-        <v>343052</v>
+        <v>103050</v>
       </c>
       <c r="C7" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!C$1)</f>
-        <v>698432</v>
+        <v>579786</v>
       </c>
       <c r="D7" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!D$1)</f>
-        <v>700448</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>512804</v>
+      </c>
+      <c r="E7" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
       <c r="F7" s="2">
-        <f>SUM(B7:D7)</f>
-        <v>1741932</v>
-      </c>
-      <c r="G7" s="9">
-        <v>2018</v>
-      </c>
-      <c r="H7" s="11">
-        <f>F7-F8</f>
-        <v>480441</v>
-      </c>
-      <c r="I7" s="16">
-        <f t="shared" ref="I7:I14" si="12">B7-B8</f>
-        <v>216252</v>
-      </c>
-      <c r="J7" s="16">
-        <f t="shared" ref="J7:J14" si="13">C7-C8</f>
-        <v>146054</v>
-      </c>
-      <c r="K7" s="16">
-        <f t="shared" ref="K7:K14" si="14">D7-D8</f>
-        <v>118135</v>
-      </c>
-      <c r="L7" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1195640</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2012</v>
+      </c>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!B$1)</f>
-        <v>126800</v>
+        <v>103050</v>
       </c>
       <c r="C8" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!C$1)</f>
-        <v>552378</v>
+        <v>474063</v>
       </c>
       <c r="D8" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!D$1)</f>
-        <v>582313</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>541051</v>
+      </c>
+      <c r="E8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
       <c r="F8" s="2">
-        <f>SUM(B8:D8)</f>
-        <v>1261491</v>
+        <f t="shared" si="0"/>
+        <v>1118164</v>
       </c>
       <c r="G8" s="10">
-        <v>2017</v>
-      </c>
-      <c r="H8" s="11">
-        <f t="shared" ref="H8:H14" si="15">F8-F9</f>
-        <v>511813</v>
-      </c>
-      <c r="I8" s="16">
-        <f t="shared" si="12"/>
-        <v>23750</v>
-      </c>
-      <c r="J8" s="16">
-        <f t="shared" si="13"/>
-        <v>437312</v>
-      </c>
-      <c r="K8" s="16">
-        <f t="shared" si="14"/>
-        <v>50751</v>
-      </c>
-      <c r="L8" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!B$1)</f>
@@ -1196,42 +1061,25 @@
       </c>
       <c r="C9" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!C$1)</f>
-        <v>115066</v>
+        <v>169085</v>
       </c>
       <c r="D9" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!D$1)</f>
-        <v>531562</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>564765</v>
+      </c>
+      <c r="E9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
       <c r="F9" s="2">
-        <f t="shared" ref="F9:F18" si="16">SUM(B9:D9)</f>
-        <v>749678</v>
+        <f t="shared" si="0"/>
+        <v>836900</v>
       </c>
       <c r="G9" s="10">
-        <v>2016</v>
-      </c>
-      <c r="H9" s="11">
-        <f t="shared" si="15"/>
-        <v>37814</v>
-      </c>
-      <c r="I9" s="16">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="16">
-        <f t="shared" si="13"/>
-        <v>17275</v>
-      </c>
-      <c r="K9" s="16">
-        <f t="shared" si="14"/>
-        <v>20539</v>
-      </c>
-      <c r="L9" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1247,38 +1095,21 @@
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G10,'By User'!$C$2:$C$43,Balances!D$1)</f>
         <v>511023</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G10,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
       <c r="F10" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>711864</v>
       </c>
       <c r="G10" s="10">
         <v>2015</v>
       </c>
-      <c r="H10" s="11">
-        <f t="shared" si="15"/>
-        <v>-125036</v>
-      </c>
-      <c r="I10" s="16">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="16">
-        <f t="shared" si="13"/>
-        <v>-71294</v>
-      </c>
-      <c r="K10" s="16">
-        <f t="shared" si="14"/>
-        <v>-53742</v>
-      </c>
-      <c r="L10" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!B$1)</f>
@@ -1286,347 +1117,712 @@
       </c>
       <c r="C11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!C$1)</f>
-        <v>169085</v>
+        <v>115066</v>
       </c>
       <c r="D11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!D$1)</f>
-        <v>564765</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>531562</v>
+      </c>
+      <c r="E11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
       <c r="F11" s="2">
-        <f t="shared" si="16"/>
-        <v>836900</v>
+        <f t="shared" si="0"/>
+        <v>749678</v>
       </c>
       <c r="G11" s="10">
-        <v>2014</v>
-      </c>
-      <c r="H11" s="11">
-        <f t="shared" si="15"/>
-        <v>-281264</v>
-      </c>
-      <c r="I11" s="16">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="16">
-        <f t="shared" si="13"/>
-        <v>-304978</v>
-      </c>
-      <c r="K11" s="16">
-        <f t="shared" si="14"/>
-        <v>23714</v>
-      </c>
-      <c r="L11" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!B$1)</f>
-        <v>103050</v>
+        <v>126800</v>
       </c>
       <c r="C12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!C$1)</f>
-        <v>474063</v>
+        <v>552378</v>
       </c>
       <c r="D12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!D$1)</f>
-        <v>541051</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>582313</v>
+      </c>
+      <c r="E12" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
       <c r="F12" s="2">
-        <f t="shared" si="16"/>
-        <v>1118164</v>
+        <f t="shared" si="0"/>
+        <v>1261491</v>
       </c>
       <c r="G12" s="10">
-        <v>2013</v>
-      </c>
-      <c r="H12" s="11">
-        <f t="shared" si="15"/>
-        <v>-77476</v>
-      </c>
-      <c r="I12" s="16">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="16">
-        <f t="shared" si="13"/>
-        <v>-105723</v>
-      </c>
-      <c r="K12" s="16">
-        <f t="shared" si="14"/>
-        <v>28247</v>
-      </c>
-      <c r="L12" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!B$1)</f>
-        <v>103050</v>
+        <v>343052</v>
       </c>
       <c r="C13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!C$1)</f>
-        <v>579786</v>
+        <v>698432</v>
       </c>
       <c r="D13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!D$1)</f>
-        <v>512804</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>700448</v>
+      </c>
+      <c r="E13" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
       <c r="F13" s="2">
-        <f t="shared" si="16"/>
-        <v>1195640</v>
-      </c>
-      <c r="G13" s="10">
-        <v>2012</v>
-      </c>
-      <c r="H13" s="11">
-        <f t="shared" si="15"/>
-        <v>169240</v>
-      </c>
-      <c r="I13" s="16">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="16">
-        <f t="shared" si="13"/>
-        <v>139108</v>
-      </c>
-      <c r="K13" s="16">
-        <f t="shared" si="14"/>
-        <v>30132</v>
-      </c>
-      <c r="L13" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1741932</v>
+      </c>
+      <c r="G13" s="9">
+        <v>2018</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!B$1)</f>
-        <v>103050</v>
+        <v>473504</v>
       </c>
       <c r="C14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!C$1)</f>
-        <v>440678</v>
+        <v>1053210</v>
       </c>
       <c r="D14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!D$1)</f>
-        <v>482672</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>785913</v>
+      </c>
+      <c r="E14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
       <c r="F14" s="2">
-        <f t="shared" si="16"/>
-        <v>1026400</v>
-      </c>
-      <c r="G14" s="10">
+        <f t="shared" si="0"/>
+        <v>2312627</v>
+      </c>
+      <c r="G14" s="12">
+        <v>2019</v>
+      </c>
+      <c r="H14" s="11">
+        <f>SUM(E14:F14)</f>
+        <v>2312627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="16">
+        <v>598742</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1375871</v>
+      </c>
+      <c r="D15" s="16">
+        <v>865741</v>
+      </c>
+      <c r="E15" s="16">
+        <f>41000+E16</f>
+        <v>78000</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>2840354</v>
+      </c>
+      <c r="G15" s="17">
+        <v>2020</v>
+      </c>
+      <c r="H15" s="11">
+        <f>SUM(E15:F15)</f>
+        <v>2918354</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="16">
+        <v>684201</v>
+      </c>
+      <c r="C16" s="16">
+        <v>1357085</v>
+      </c>
+      <c r="D16" s="16">
+        <v>949658</v>
+      </c>
+      <c r="E16" s="16">
+        <f>41000+E17</f>
+        <v>37000</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>2990944</v>
+      </c>
+      <c r="G16" s="17">
+        <v>2021</v>
+      </c>
+      <c r="H16" s="11">
+        <f>SUM(E16:F16)</f>
+        <v>3027944</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="16">
+        <v>753423</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1245693</v>
+      </c>
+      <c r="D17" s="16">
+        <v>1038765</v>
+      </c>
+      <c r="E17" s="16">
+        <f>30000+E18</f>
+        <v>-4000</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>3037881</v>
+      </c>
+      <c r="G17" s="17">
+        <v>2022</v>
+      </c>
+      <c r="H17" s="11">
+        <f>SUM(E17:F17)</f>
+        <v>3033881</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="23">
+        <v>710589</v>
+      </c>
+      <c r="C18" s="23">
+        <v>1661832</v>
+      </c>
+      <c r="D18" s="23">
+        <v>955543</v>
+      </c>
+      <c r="E18" s="18">
+        <f>E19-34000</f>
+        <v>-34000</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>3327964</v>
+      </c>
+      <c r="G18" s="12">
+        <v>2023</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H18">
+    <sortCondition ref="G2:G18"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C452AE-E84E-4682-A6B7-6BBA39D2CE31}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="12"/>
+    <col min="2" max="2" width="11.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.1796875" style="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="str" cm="1">
+        <f t="array" ref="A1">Balances!G1:G1</f>
+        <v>Year</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="12">
+        <f>Balances!G2</f>
+        <v>2007</v>
+      </c>
+      <c r="B2" s="16">
+        <f>SUM(C2:F2)</f>
+        <v>41398</v>
+      </c>
+      <c r="C2" s="16">
+        <f>Balances!B2</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="16">
+        <f>Balances!C2</f>
+        <v>41398</v>
+      </c>
+      <c r="E2" s="16">
+        <f>Balances!D2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="16">
+        <f>Balances!E3-Balances!E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
+        <f>Balances!G3</f>
+        <v>2008</v>
+      </c>
+      <c r="B3" s="16">
+        <f t="shared" ref="B3:B18" si="0">SUM(C3:F3)</f>
+        <v>552175</v>
+      </c>
+      <c r="C3" s="16">
+        <f>Balances!B3-Balances!B2</f>
+        <v>100000</v>
+      </c>
+      <c r="D3" s="16">
+        <f>Balances!C3-Balances!C2</f>
+        <v>52175</v>
+      </c>
+      <c r="E3" s="16">
+        <f>Balances!D3-Balances!D2</f>
+        <v>400000</v>
+      </c>
+      <c r="F3" s="16">
+        <f>Balances!E3-Balances!E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
+        <f>Balances!G4</f>
+        <v>2009</v>
+      </c>
+      <c r="B4" s="16">
+        <f t="shared" si="0"/>
+        <v>63617</v>
+      </c>
+      <c r="C4" s="16">
+        <f>Balances!B4-Balances!B3</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="16">
+        <f>Balances!C4-Balances!C3</f>
+        <v>63617</v>
+      </c>
+      <c r="E4" s="16">
+        <f>Balances!D4-Balances!D3</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="16">
+        <f>Balances!E4-Balances!E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="12">
+        <f>Balances!G5</f>
+        <v>2010</v>
+      </c>
+      <c r="B5" s="16">
+        <f t="shared" si="0"/>
+        <v>158151</v>
+      </c>
+      <c r="C5" s="16">
+        <f>Balances!B5-Balances!B4</f>
+        <v>2094</v>
+      </c>
+      <c r="D5" s="16">
+        <f>Balances!C5-Balances!C4</f>
+        <v>104800</v>
+      </c>
+      <c r="E5" s="16">
+        <f>Balances!D5-Balances!D4</f>
+        <v>51257</v>
+      </c>
+      <c r="F5" s="16">
+        <f>Balances!E5-Balances!E4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
+        <f>Balances!G6</f>
         <v>2011</v>
       </c>
-      <c r="H14" s="11">
-        <f t="shared" si="15"/>
+      <c r="B6" s="16">
+        <f t="shared" si="0"/>
         <v>211059</v>
       </c>
-      <c r="I14" s="16">
-        <f t="shared" si="12"/>
+      <c r="C6" s="16">
+        <f>Balances!B6-Balances!B5</f>
         <v>956</v>
       </c>
-      <c r="J14" s="16">
-        <f t="shared" si="13"/>
+      <c r="D6" s="16">
+        <f>Balances!C6-Balances!C5</f>
         <v>178688</v>
       </c>
-      <c r="K14" s="16">
-        <f t="shared" si="14"/>
+      <c r="E6" s="16">
+        <f>Balances!D6-Balances!D5</f>
         <v>31415</v>
       </c>
-      <c r="L14" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G15,'By User'!$C$2:$C$43,Balances!B$1)</f>
-        <v>102094</v>
-      </c>
-      <c r="C15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G15,'By User'!$C$2:$C$43,Balances!C$1)</f>
-        <v>261990</v>
-      </c>
-      <c r="D15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G15,'By User'!$C$2:$C$43,Balances!D$1)</f>
-        <v>451257</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2">
-        <f t="shared" si="16"/>
-        <v>815341</v>
-      </c>
-      <c r="G15" s="10">
-        <v>2010</v>
-      </c>
-      <c r="H15" s="11">
-        <f t="shared" ref="H15:H18" si="17">F15-F16</f>
-        <v>158151</v>
-      </c>
-      <c r="I15" s="16">
-        <f t="shared" ref="I15:I18" si="18">B15-B16</f>
-        <v>2094</v>
-      </c>
-      <c r="J15" s="16">
-        <f t="shared" ref="J15:J18" si="19">C15-C16</f>
-        <v>104800</v>
-      </c>
-      <c r="K15" s="16">
-        <f t="shared" ref="K15:K18" si="20">D15-D16</f>
-        <v>51257</v>
-      </c>
-      <c r="L15" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="2">
-        <v>100000</v>
-      </c>
-      <c r="C16" s="2">
-        <f>79790+66000+11400</f>
-        <v>157190</v>
-      </c>
-      <c r="D16" s="2">
-        <v>400000</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2">
-        <f t="shared" si="16"/>
-        <v>657190</v>
-      </c>
-      <c r="G16" s="10">
-        <v>2009</v>
-      </c>
-      <c r="H16" s="11">
-        <f t="shared" si="17"/>
-        <v>63617</v>
-      </c>
-      <c r="I16" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="16">
-        <f t="shared" si="19"/>
-        <v>63617</v>
-      </c>
-      <c r="K16" s="16">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="2">
-        <v>100000</v>
-      </c>
-      <c r="C17" s="2">
-        <f>27573+66000</f>
-        <v>93573</v>
-      </c>
-      <c r="D17" s="2">
-        <v>400000</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2">
-        <f t="shared" si="16"/>
-        <v>593573</v>
-      </c>
-      <c r="G17" s="10">
-        <v>2008</v>
-      </c>
-      <c r="H17" s="11">
-        <f t="shared" si="17"/>
-        <v>552175</v>
-      </c>
-      <c r="I17" s="16">
-        <f t="shared" si="18"/>
-        <v>100000</v>
-      </c>
-      <c r="J17" s="16">
-        <f t="shared" si="19"/>
-        <v>52175</v>
-      </c>
-      <c r="K17" s="16">
-        <f t="shared" si="20"/>
-        <v>400000</v>
-      </c>
-      <c r="L17" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>41398</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2">
-        <f t="shared" si="16"/>
-        <v>41398</v>
-      </c>
-      <c r="G18" s="10">
-        <v>2007</v>
-      </c>
-      <c r="H18" s="11">
-        <f t="shared" si="17"/>
-        <v>41398</v>
-      </c>
-      <c r="I18" s="16">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="16">
-        <f t="shared" si="19"/>
-        <v>41398</v>
-      </c>
-      <c r="K18" s="16">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="16">
-        <f t="shared" si="11"/>
-        <v>0</v>
+      <c r="F6" s="16">
+        <f>Balances!E6-Balances!E5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
+        <f>Balances!G7</f>
+        <v>2012</v>
+      </c>
+      <c r="B7" s="16">
+        <f t="shared" si="0"/>
+        <v>169240</v>
+      </c>
+      <c r="C7" s="16">
+        <f>Balances!B7-Balances!B6</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <f>Balances!C7-Balances!C6</f>
+        <v>139108</v>
+      </c>
+      <c r="E7" s="16">
+        <f>Balances!D7-Balances!D6</f>
+        <v>30132</v>
+      </c>
+      <c r="F7" s="16">
+        <f>Balances!E7-Balances!E6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
+        <f>Balances!G8</f>
+        <v>2013</v>
+      </c>
+      <c r="B8" s="16">
+        <f t="shared" si="0"/>
+        <v>-77476</v>
+      </c>
+      <c r="C8" s="16">
+        <f>Balances!B8-Balances!B7</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="16">
+        <f>Balances!C8-Balances!C7</f>
+        <v>-105723</v>
+      </c>
+      <c r="E8" s="16">
+        <f>Balances!D8-Balances!D7</f>
+        <v>28247</v>
+      </c>
+      <c r="F8" s="16">
+        <f>Balances!E8-Balances!E7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="12">
+        <f>Balances!G9</f>
+        <v>2014</v>
+      </c>
+      <c r="B9" s="16">
+        <f t="shared" si="0"/>
+        <v>-281264</v>
+      </c>
+      <c r="C9" s="16">
+        <f>Balances!B9-Balances!B8</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="16">
+        <f>Balances!C9-Balances!C8</f>
+        <v>-304978</v>
+      </c>
+      <c r="E9" s="16">
+        <f>Balances!D9-Balances!D8</f>
+        <v>23714</v>
+      </c>
+      <c r="F9" s="16">
+        <f>Balances!E9-Balances!E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="12">
+        <f>Balances!G10</f>
+        <v>2015</v>
+      </c>
+      <c r="B10" s="16">
+        <f t="shared" si="0"/>
+        <v>-125036</v>
+      </c>
+      <c r="C10" s="16">
+        <f>Balances!B10-Balances!B9</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="16">
+        <f>Balances!C10-Balances!C9</f>
+        <v>-71294</v>
+      </c>
+      <c r="E10" s="16">
+        <f>Balances!D10-Balances!D9</f>
+        <v>-53742</v>
+      </c>
+      <c r="F10" s="16">
+        <f>Balances!E10-Balances!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="12">
+        <f>Balances!G11</f>
+        <v>2016</v>
+      </c>
+      <c r="B11" s="16">
+        <f t="shared" si="0"/>
+        <v>37814</v>
+      </c>
+      <c r="C11" s="16">
+        <f>Balances!B11-Balances!B10</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="16">
+        <f>Balances!C11-Balances!C10</f>
+        <v>17275</v>
+      </c>
+      <c r="E11" s="16">
+        <f>Balances!D11-Balances!D10</f>
+        <v>20539</v>
+      </c>
+      <c r="F11" s="16">
+        <f>Balances!E11-Balances!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="12">
+        <f>Balances!G12</f>
+        <v>2017</v>
+      </c>
+      <c r="B12" s="16">
+        <f t="shared" si="0"/>
+        <v>511813</v>
+      </c>
+      <c r="C12" s="16">
+        <f>Balances!B12-Balances!B11</f>
+        <v>23750</v>
+      </c>
+      <c r="D12" s="16">
+        <f>Balances!C12-Balances!C11</f>
+        <v>437312</v>
+      </c>
+      <c r="E12" s="16">
+        <f>Balances!D12-Balances!D11</f>
+        <v>50751</v>
+      </c>
+      <c r="F12" s="16">
+        <f>Balances!E12-Balances!E11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="12">
+        <f>Balances!G13</f>
+        <v>2018</v>
+      </c>
+      <c r="B13" s="16">
+        <f t="shared" si="0"/>
+        <v>480441</v>
+      </c>
+      <c r="C13" s="16">
+        <f>Balances!B13-Balances!B12</f>
+        <v>216252</v>
+      </c>
+      <c r="D13" s="16">
+        <f>Balances!C13-Balances!C12</f>
+        <v>146054</v>
+      </c>
+      <c r="E13" s="16">
+        <f>Balances!D13-Balances!D12</f>
+        <v>118135</v>
+      </c>
+      <c r="F13" s="16">
+        <f>Balances!E13-Balances!E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="12">
+        <f>Balances!G14</f>
+        <v>2019</v>
+      </c>
+      <c r="B14" s="16">
+        <f t="shared" si="0"/>
+        <v>570695</v>
+      </c>
+      <c r="C14" s="16">
+        <f>Balances!B14-Balances!B13</f>
+        <v>130452</v>
+      </c>
+      <c r="D14" s="16">
+        <f>Balances!C14-Balances!C13</f>
+        <v>354778</v>
+      </c>
+      <c r="E14" s="16">
+        <f>Balances!D14-Balances!D13</f>
+        <v>85465</v>
+      </c>
+      <c r="F14" s="16">
+        <f>Balances!E14-Balances!E13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
+        <f>Balances!G15</f>
+        <v>2020</v>
+      </c>
+      <c r="B15" s="16">
+        <f t="shared" si="0"/>
+        <v>605727</v>
+      </c>
+      <c r="C15" s="16">
+        <f>Balances!B15-Balances!B14</f>
+        <v>125238</v>
+      </c>
+      <c r="D15" s="16">
+        <f>Balances!C15-Balances!C14</f>
+        <v>322661</v>
+      </c>
+      <c r="E15" s="16">
+        <f>Balances!D15-Balances!D14</f>
+        <v>79828</v>
+      </c>
+      <c r="F15" s="16">
+        <f>Balances!E15-Balances!E14</f>
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="12">
+        <f>Balances!G16</f>
+        <v>2021</v>
+      </c>
+      <c r="B16" s="16">
+        <f t="shared" si="0"/>
+        <v>109590</v>
+      </c>
+      <c r="C16" s="16">
+        <f>Balances!B16-Balances!B15</f>
+        <v>85459</v>
+      </c>
+      <c r="D16" s="16">
+        <f>Balances!C16-Balances!C15</f>
+        <v>-18786</v>
+      </c>
+      <c r="E16" s="16">
+        <f>Balances!D16-Balances!D15</f>
+        <v>83917</v>
+      </c>
+      <c r="F16" s="16">
+        <f>Balances!E16-Balances!E15</f>
+        <v>-41000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="12">
+        <f>Balances!G17</f>
+        <v>2022</v>
+      </c>
+      <c r="B17" s="16">
+        <f t="shared" si="0"/>
+        <v>5937</v>
+      </c>
+      <c r="C17" s="16">
+        <f>Balances!B17-Balances!B16</f>
+        <v>69222</v>
+      </c>
+      <c r="D17" s="16">
+        <f>Balances!C17-Balances!C16</f>
+        <v>-111392</v>
+      </c>
+      <c r="E17" s="16">
+        <f>Balances!D17-Balances!D16</f>
+        <v>89107</v>
+      </c>
+      <c r="F17" s="16">
+        <f>Balances!E17-Balances!E16</f>
+        <v>-41000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="12">
+        <f>Balances!G18</f>
+        <v>2023</v>
+      </c>
+      <c r="B18" s="16">
+        <f t="shared" si="0"/>
+        <v>260083</v>
+      </c>
+      <c r="C18" s="16">
+        <f>Balances!B18-Balances!B17</f>
+        <v>-42834</v>
+      </c>
+      <c r="D18" s="16">
+        <f>Balances!C18-Balances!C17</f>
+        <v>416139</v>
+      </c>
+      <c r="E18" s="16">
+        <f>Balances!D18-Balances!D17</f>
+        <v>-83222</v>
+      </c>
+      <c r="F18" s="16">
+        <f>Balances!E18-Balances!E17</f>
+        <v>-30000</v>
       </c>
     </row>
   </sheetData>
@@ -1634,7 +1830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9C09D6-2BEE-4EAC-9C47-48919B4DAC3E}">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -1829,14 +2025,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1898,7 +2094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -1914,11 +2110,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
@@ -1988,12 +2184,12 @@
       </c>
       <c r="E7" s="15">
         <f>Balances!B$5/B7</f>
-        <v>3.1184479166666668</v>
+        <v>0.53173958333333338</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15">
         <f>Balances!D$5/D7</f>
-        <v>108.217625</v>
+        <v>56.407125000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -2009,12 +2205,12 @@
       </c>
       <c r="E8" s="15">
         <f>Balances!B$5/B8</f>
-        <v>1.1694179687499999</v>
+        <v>0.19940234374999999</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15">
         <f>Balances!D$5/D8</f>
-        <v>41.225761904761903</v>
+        <v>21.488428571428571</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -2030,12 +2226,12 @@
       </c>
       <c r="E9" s="15">
         <f>Balances!B$5/B9</f>
-        <v>1.0113885135135134</v>
+        <v>0.17245608108108107</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15">
         <f>Balances!D$5/D9</f>
-        <v>34.629640000000002</v>
+        <v>18.050280000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -2053,15 +2249,15 @@
       </c>
       <c r="E10" s="15">
         <f>Balances!B$5/B10</f>
-        <v>0.93553437500000003</v>
+        <v>0.15952187500000001</v>
       </c>
       <c r="F10" s="15">
         <f>Balances!C$5/C10</f>
-        <v>6.8793550000000003</v>
+        <v>1.3099499999999999</v>
       </c>
       <c r="G10" s="15">
         <f>Balances!D$5/D10</f>
-        <v>32.064481481481479</v>
+        <v>16.713222222222221</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -2079,15 +2275,15 @@
       </c>
       <c r="E11" s="15">
         <f>Balances!B$5/B11</f>
-        <v>0.93553437500000003</v>
+        <v>0.15952187500000001</v>
       </c>
       <c r="F11" s="15">
         <f>Balances!C$5/C11</f>
-        <v>5.5034840000000003</v>
+        <v>1.04796</v>
       </c>
       <c r="G11" s="15">
         <f>Balances!D$5/D11</f>
-        <v>32.064481481481479</v>
+        <v>16.713222222222221</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -2105,15 +2301,15 @@
       </c>
       <c r="E12" s="15">
         <f>Balances!B$5/B12</f>
-        <v>0.93553437500000003</v>
+        <v>0.15952187500000001</v>
       </c>
       <c r="F12" s="15">
         <f>Balances!C$5/C12</f>
-        <v>4.5862366666666663</v>
+        <v>0.87329999999999997</v>
       </c>
       <c r="G12" s="15">
         <f>Balances!D$5/D12</f>
-        <v>32.064481481481479</v>
+        <v>16.713222222222221</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -2131,15 +2327,15 @@
       </c>
       <c r="E13" s="15">
         <f>Balances!B$5/B13</f>
-        <v>0.93553437500000003</v>
+        <v>0.15952187500000001</v>
       </c>
       <c r="F13" s="15">
         <f>Balances!C$5/C13</f>
-        <v>3.93106</v>
+        <v>0.74854285714285718</v>
       </c>
       <c r="G13" s="15">
         <f>Balances!D$5/D13</f>
-        <v>32.064481481481479</v>
+        <v>16.713222222222221</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -2157,15 +2353,15 @@
       </c>
       <c r="E14" s="15">
         <f>Balances!B$5/B14</f>
-        <v>0.83158611111111114</v>
+        <v>0.14179722222222221</v>
       </c>
       <c r="F14" s="15">
         <f>Balances!C$5/C14</f>
-        <v>3.93106</v>
+        <v>0.74854285714285718</v>
       </c>
       <c r="G14" s="15">
         <f>Balances!D$5/D14</f>
-        <v>28.858033333333335</v>
+        <v>15.0419</v>
       </c>
     </row>
   </sheetData>
@@ -2176,7 +2372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
   <dimension ref="A2:I7"/>
   <sheetViews>
@@ -2204,22 +2400,22 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>51</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>53</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>54</v>
-      </c>
-      <c r="I2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2227,7 +2423,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>2020</v>
@@ -2319,7 +2515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>

</xml_diff>

<commit_message>
Read from ICS Balances worksheet without row numbers
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B7E62C-357D-49C9-BF3C-523C1106752D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACF12E2-AA49-4594-8D0D-8D62EF378416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
@@ -442,13 +442,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -830,11 +830,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -887,15 +887,20 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
       <c r="F2" s="2">
-        <f t="shared" ref="F2:F18" si="0">SUM(B2:D2)</f>
+        <f>SUM(B2:E2)</f>
         <v>41398</v>
       </c>
       <c r="G2" s="10">
         <v>2007</v>
       </c>
-      <c r="H2"/>
+      <c r="H2" s="11">
+        <f t="shared" ref="H2:H13" si="0">SUM(E2:F2)</f>
+        <v>41398</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -911,13 +916,19 @@
       <c r="D3" s="2">
         <v>400000</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
       <c r="F3" s="2">
+        <f t="shared" ref="F3:F18" si="1">SUM(B3:D3)</f>
+        <v>593573</v>
+      </c>
+      <c r="G3" s="10">
+        <v>2008</v>
+      </c>
+      <c r="H3" s="11">
         <f t="shared" si="0"/>
         <v>593573</v>
-      </c>
-      <c r="G3" s="10">
-        <v>2008</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -934,13 +945,19 @@
       <c r="D4" s="2">
         <v>400000</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
       <c r="F4" s="2">
+        <f t="shared" si="1"/>
+        <v>657190</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2009</v>
+      </c>
+      <c r="H4" s="11">
         <f t="shared" si="0"/>
         <v>657190</v>
-      </c>
-      <c r="G4" s="10">
-        <v>2009</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -956,13 +973,19 @@
       <c r="D5" s="2">
         <v>451257</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
       <c r="F5" s="2">
+        <f>SUM(B5:E5)</f>
+        <v>815341</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2010</v>
+      </c>
+      <c r="H5" s="11">
         <f t="shared" si="0"/>
         <v>815341</v>
-      </c>
-      <c r="G5" s="10">
-        <v>2010</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -986,13 +1009,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>1026400</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2011</v>
+      </c>
+      <c r="H6" s="11">
         <f t="shared" si="0"/>
         <v>1026400</v>
       </c>
-      <c r="G6" s="10">
-        <v>2011</v>
-      </c>
-      <c r="H6"/>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1015,13 +1041,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>1195640</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2012</v>
+      </c>
+      <c r="H7" s="11">
         <f t="shared" si="0"/>
         <v>1195640</v>
       </c>
-      <c r="G7" s="10">
-        <v>2012</v>
-      </c>
-      <c r="H7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1044,11 +1073,15 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>1118164</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2013</v>
+      </c>
+      <c r="H8" s="11">
         <f t="shared" si="0"/>
         <v>1118164</v>
-      </c>
-      <c r="G8" s="10">
-        <v>2013</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1072,11 +1105,15 @@
         <v>0</v>
       </c>
       <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>836900</v>
+      </c>
+      <c r="G9" s="10">
+        <v>2014</v>
+      </c>
+      <c r="H9" s="11">
         <f t="shared" si="0"/>
         <v>836900</v>
-      </c>
-      <c r="G9" s="10">
-        <v>2014</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1100,11 +1137,15 @@
         <v>0</v>
       </c>
       <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>711864</v>
+      </c>
+      <c r="G10" s="10">
+        <v>2015</v>
+      </c>
+      <c r="H10" s="11">
         <f t="shared" si="0"/>
         <v>711864</v>
-      </c>
-      <c r="G10" s="10">
-        <v>2015</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1128,11 +1169,15 @@
         <v>0</v>
       </c>
       <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>749678</v>
+      </c>
+      <c r="G11" s="10">
+        <v>2016</v>
+      </c>
+      <c r="H11" s="11">
         <f t="shared" si="0"/>
         <v>749678</v>
-      </c>
-      <c r="G11" s="10">
-        <v>2016</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1156,11 +1201,15 @@
         <v>0</v>
       </c>
       <c r="F12" s="2">
+        <f t="shared" si="1"/>
+        <v>1261491</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2017</v>
+      </c>
+      <c r="H12" s="11">
         <f t="shared" si="0"/>
         <v>1261491</v>
-      </c>
-      <c r="G12" s="10">
-        <v>2017</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1184,13 +1233,16 @@
         <v>0</v>
       </c>
       <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>1741932</v>
+      </c>
+      <c r="G13" s="9">
+        <v>2018</v>
+      </c>
+      <c r="H13" s="11">
         <f t="shared" si="0"/>
         <v>1741932</v>
       </c>
-      <c r="G13" s="9">
-        <v>2018</v>
-      </c>
-      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1209,11 +1261,10 @@
         <v>785913</v>
       </c>
       <c r="E14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!E$1)</f>
-        <v>0</v>
+        <v>132975</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2312627</v>
       </c>
       <c r="G14" s="12">
@@ -1221,7 +1272,7 @@
       </c>
       <c r="H14" s="11">
         <f>SUM(E14:F14)</f>
-        <v>2312627</v>
+        <v>2445602</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1238,11 +1289,11 @@
         <v>865741</v>
       </c>
       <c r="E15" s="16">
-        <f>41000+E16</f>
-        <v>78000</v>
+        <f>E14+41000</f>
+        <v>173975</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2840354</v>
       </c>
       <c r="G15" s="17">
@@ -1250,7 +1301,7 @@
       </c>
       <c r="H15" s="11">
         <f>SUM(E15:F15)</f>
-        <v>2918354</v>
+        <v>3014329</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1267,11 +1318,11 @@
         <v>949658</v>
       </c>
       <c r="E16" s="16">
-        <f>41000+E17</f>
-        <v>37000</v>
+        <f>E15+41000</f>
+        <v>214975</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2990944</v>
       </c>
       <c r="G16" s="17">
@@ -1279,7 +1330,7 @@
       </c>
       <c r="H16" s="11">
         <f>SUM(E16:F16)</f>
-        <v>3027944</v>
+        <v>3205919</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1296,11 +1347,11 @@
         <v>1038765</v>
       </c>
       <c r="E17" s="16">
-        <f>30000+E18</f>
-        <v>-4000</v>
+        <f>30000+E16</f>
+        <v>244975</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3037881</v>
       </c>
       <c r="G17" s="17">
@@ -1308,34 +1359,37 @@
       </c>
       <c r="H17" s="11">
         <f>SUM(E17:F17)</f>
-        <v>3033881</v>
+        <v>3282856</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="21">
         <v>710589</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="21">
         <v>1661832</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="21">
         <v>955543</v>
       </c>
       <c r="E18" s="18">
-        <f>E19-34000</f>
-        <v>-34000</v>
+        <f>E17-34000</f>
+        <v>210975</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3327964</v>
       </c>
       <c r="G18" s="12">
         <v>2023</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="11">
+        <f>SUM(E18:F18)</f>
+        <v>3538939</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H18">
@@ -1349,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C452AE-E84E-4682-A6B7-6BBA39D2CE31}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1702,7 +1756,7 @@
       </c>
       <c r="B14" s="16">
         <f t="shared" si="0"/>
-        <v>570695</v>
+        <v>703670</v>
       </c>
       <c r="C14" s="16">
         <f>Balances!B14-Balances!B13</f>
@@ -1718,7 +1772,7 @@
       </c>
       <c r="F14" s="16">
         <f>Balances!E14-Balances!E13</f>
-        <v>0</v>
+        <v>132975</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1728,7 +1782,7 @@
       </c>
       <c r="B15" s="16">
         <f t="shared" si="0"/>
-        <v>605727</v>
+        <v>568727</v>
       </c>
       <c r="C15" s="16">
         <f>Balances!B15-Balances!B14</f>
@@ -1744,7 +1798,7 @@
       </c>
       <c r="F15" s="16">
         <f>Balances!E15-Balances!E14</f>
-        <v>78000</v>
+        <v>41000</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1754,7 +1808,7 @@
       </c>
       <c r="B16" s="16">
         <f t="shared" si="0"/>
-        <v>109590</v>
+        <v>191590</v>
       </c>
       <c r="C16" s="16">
         <f>Balances!B16-Balances!B15</f>
@@ -1770,7 +1824,7 @@
       </c>
       <c r="F16" s="16">
         <f>Balances!E16-Balances!E15</f>
-        <v>-41000</v>
+        <v>41000</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1780,7 +1834,7 @@
       </c>
       <c r="B17" s="16">
         <f t="shared" si="0"/>
-        <v>5937</v>
+        <v>76937</v>
       </c>
       <c r="C17" s="16">
         <f>Balances!B17-Balances!B16</f>
@@ -1796,7 +1850,7 @@
       </c>
       <c r="F17" s="16">
         <f>Balances!E17-Balances!E16</f>
-        <v>-41000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1806,7 +1860,7 @@
       </c>
       <c r="B18" s="16">
         <f t="shared" si="0"/>
-        <v>260083</v>
+        <v>256083</v>
       </c>
       <c r="C18" s="16">
         <f>Balances!B18-Balances!B17</f>
@@ -1822,7 +1876,7 @@
       </c>
       <c r="F18" s="16">
         <f>Balances!E18-Balances!E17</f>
-        <v>-30000</v>
+        <v>-34000</v>
       </c>
     </row>
   </sheetData>
@@ -2025,14 +2079,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -2110,11 +2164,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">

</xml_diff>